<commit_message>
added more tests from laptop
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7EBC94-32D2-42DA-8C46-DDFBC7FF7265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A7D31-BF80-434A-82FE-FA3897C7F343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="23">
   <si>
     <t>test number</t>
   </si>
@@ -102,17 +102,60 @@
     <t>sound clips</t>
   </si>
   <si>
-    <t>NEXT TASK: create a model that gets trained on only 10 folders, but ALL the files from those folders.</t>
-  </si>
-  <si>
-    <t>THEN: extend that to 25 folders, and compare</t>
+    <r>
+      <t xml:space="preserve">changed method to look at 10 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">full </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>folders</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tested on LAPTOP.
+Peaked at 53% test acc.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +179,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -168,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,6 +238,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,8 +455,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:Q34" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A2:Q34" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:Q41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A2:Q41" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q32">
     <sortCondition ref="A2:A32"/>
   </sortState>
@@ -430,9 +484,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -470,7 +524,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -576,7 +630,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -718,7 +772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +804,7 @@
     <col min="14" max="14" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2296,7 +2350,7 @@
       <c r="F32" s="4">
         <v>4717</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="1">
         <v>1000</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -2327,44 +2381,44 @@
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="1">
         <v>25</v>
       </c>
-      <c r="C33" s="6">
-        <v>2</v>
-      </c>
-      <c r="D33" s="6">
-        <v>200</v>
-      </c>
-      <c r="E33" s="6">
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>200</v>
+      </c>
+      <c r="E33" s="1">
         <v>0.3</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="1">
         <v>4717</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="1">
         <v>1000</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="6" t="s">
+      <c r="H33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J33" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K33" s="6">
-        <v>0</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
         <v>0.2</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="1">
         <v>32</v>
       </c>
       <c r="N33" s="2">
@@ -2377,38 +2431,38 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="1">
         <v>25</v>
       </c>
-      <c r="C34" s="6">
-        <v>2</v>
-      </c>
-      <c r="D34" s="6">
-        <v>200</v>
-      </c>
-      <c r="E34" s="6">
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>200</v>
+      </c>
+      <c r="E34" s="1">
         <v>0.3</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="1">
         <v>4717</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="1">
         <v>1000</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="6">
+      <c r="H34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K34" s="1">
         <v>0</v>
       </c>
       <c r="L34" s="4">
@@ -2427,14 +2481,357 @@
         <v>270</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H36" s="1" t="s">
+    <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>31</v>
+      </c>
+      <c r="B35" s="4">
+        <v>10</v>
+      </c>
+      <c r="C35" s="6">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F35" s="4">
+        <v>14922</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0</v>
+      </c>
+      <c r="L35" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M35" s="6">
+        <v>64</v>
+      </c>
+      <c r="N35" s="2">
+        <v>67</v>
+      </c>
+      <c r="O35" s="2">
+        <v>44</v>
+      </c>
+      <c r="P35" s="2">
+        <v>967</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H37" s="1" t="s">
-        <v>23</v>
+    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6">
+        <v>10</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F36" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G36" s="4">
+        <v>200</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K36" s="6">
+        <v>0</v>
+      </c>
+      <c r="L36" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M36" s="4">
+        <v>32</v>
+      </c>
+      <c r="N36" s="2">
+        <v>58</v>
+      </c>
+      <c r="O36" s="2">
+        <v>38</v>
+      </c>
+      <c r="P36" s="2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>33</v>
+      </c>
+      <c r="B37" s="6">
+        <v>10</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F37" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G37" s="6">
+        <v>200</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K37" s="6">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <v>0</v>
+      </c>
+      <c r="M37" s="6">
+        <v>32</v>
+      </c>
+      <c r="N37" s="2">
+        <v>30</v>
+      </c>
+      <c r="O37" s="2">
+        <v>30</v>
+      </c>
+      <c r="P37" s="2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>34</v>
+      </c>
+      <c r="B38" s="6">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6">
+        <v>2</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F38" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G38" s="6">
+        <v>200</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K38" s="6">
+        <v>0</v>
+      </c>
+      <c r="L38" s="6">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4">
+        <v>64</v>
+      </c>
+      <c r="N38" s="2">
+        <v>63</v>
+      </c>
+      <c r="O38" s="2">
+        <v>40</v>
+      </c>
+      <c r="P38" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6">
+        <v>2</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F39" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G39" s="4">
+        <v>100</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K39" s="6">
+        <v>0</v>
+      </c>
+      <c r="L39" s="6">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4">
+        <v>128</v>
+      </c>
+      <c r="N39" s="2">
+        <v>56</v>
+      </c>
+      <c r="O39" s="2">
+        <v>41</v>
+      </c>
+      <c r="P39" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6">
+        <v>10</v>
+      </c>
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F40" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G40" s="6">
+        <v>100</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="K40" s="6">
+        <v>0</v>
+      </c>
+      <c r="L40" s="6">
+        <v>0</v>
+      </c>
+      <c r="M40" s="6">
+        <v>128</v>
+      </c>
+      <c r="N40" s="2">
+        <v>60</v>
+      </c>
+      <c r="O40" s="2">
+        <v>54</v>
+      </c>
+      <c r="P40" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>37</v>
+      </c>
+      <c r="B41" s="6">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6">
+        <v>2</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F41" s="6">
+        <v>14922</v>
+      </c>
+      <c r="G41" s="4">
+        <v>300</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="K41" s="6">
+        <v>0</v>
+      </c>
+      <c r="L41" s="6">
+        <v>0</v>
+      </c>
+      <c r="M41" s="6">
+        <v>128</v>
+      </c>
+      <c r="N41" s="2">
+        <v>63</v>
+      </c>
+      <c r="O41" s="2">
+        <v>49</v>
+      </c>
+      <c r="P41" s="2">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added over/undersampling to get very good results from the model on full folders
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A7D31-BF80-434A-82FE-FA3897C7F343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874E777-DF16-4DFF-90E0-34B3DF70A8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
   <si>
     <t>test number</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>batch size</t>
-  </si>
-  <si>
-    <t>folder cutoff</t>
   </si>
   <si>
     <t>gpu train time (secs)</t>
@@ -150,6 +147,28 @@
 Peaked at 53% test acc.</t>
     </r>
   </si>
+  <si>
+    <t>sound clips per file threshold</t>
+  </si>
+  <si>
+    <t>files per folder threshold</t>
+  </si>
+  <si>
+    <t>[50, 100]</t>
+  </si>
+  <si>
+    <t>applies random undersampling from files
+(deletes random ones from all classes
+except minority)</t>
+  </si>
+  <si>
+    <t>applies random oversampling from files
+(duplicates random rows from all classes
+except majority)</t>
+  </si>
+  <si>
+    <t>filtered by looking at 50-100 files per folder</t>
+  </si>
 </sst>
 </file>
 
@@ -219,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,6 +252,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,13 +262,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -455,38 +480,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:Q41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A2:Q41" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q32">
-    <sortCondition ref="A2:A32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:R45" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A2:R45" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R45">
+    <sortCondition ref="A2:A45"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="folder cutoff" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="14"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="3"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -524,7 +550,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -630,7 +656,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -772,7 +798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -780,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,44 +817,46 @@
     <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="38.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="41.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -836,52 +864,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -892,46 +923,49 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>100</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.2</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
         <v>500</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
       <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
         <v>64</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>100</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>61</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -942,46 +976,49 @@
         <v>2</v>
       </c>
       <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.2</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
         <v>500</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="4">
         <v>0.01</v>
       </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
       <c r="L4" s="1">
         <v>0</v>
       </c>
       <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <v>64</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>100</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>52</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -992,46 +1029,49 @@
         <v>2</v>
       </c>
       <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>100</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.2</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
         <v>500</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
         <v>0.3</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>64</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>98</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>68</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1042,46 +1082,49 @@
         <v>2</v>
       </c>
       <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
         <v>100</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.2</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
         <v>500</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
         <v>0.2</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>64</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>98</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>73</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1092,46 +1135,49 @@
         <v>2</v>
       </c>
       <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
         <v>100</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.2</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
         <v>500</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4">
         <v>0.01</v>
       </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
       <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>0.2</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>64</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>98</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>52</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1142,46 +1188,49 @@
         <v>2</v>
       </c>
       <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>100</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.2</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
         <v>500</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
         <v>0.1</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>64</v>
       </c>
-      <c r="N8" s="2">
-        <v>12</v>
-      </c>
       <c r="O8" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P8" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1192,46 +1241,49 @@
         <v>2</v>
       </c>
       <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
         <v>100</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.2</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
         <v>500</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4">
         <v>0.01</v>
       </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
       <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
         <v>0.1</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>64</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>100</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>63</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1242,46 +1294,49 @@
         <v>2</v>
       </c>
       <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <v>100</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.2</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
         <v>500</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
         <v>0.5</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>64</v>
       </c>
-      <c r="N10" s="2">
-        <v>12</v>
-      </c>
       <c r="O10" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P10" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1292,46 +1347,49 @@
         <v>2</v>
       </c>
       <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <v>100</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.2</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1">
         <v>500</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4">
         <v>0.01</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
       <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>0.5</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>64</v>
       </c>
-      <c r="N11" s="2">
-        <v>12</v>
-      </c>
       <c r="O11" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P11" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1342,46 +1400,49 @@
         <v>2</v>
       </c>
       <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>100</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>0.2</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1">
         <v>500</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4">
         <v>0.1</v>
       </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
       <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
         <v>0.5</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>64</v>
       </c>
-      <c r="N12" s="2">
-        <v>12</v>
-      </c>
       <c r="O12" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P12" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1392,46 +1453,49 @@
         <v>2</v>
       </c>
       <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>100</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>0.2</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1">
         <v>500</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
         <v>0.25</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>64</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>98</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>68</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1441,47 +1505,50 @@
       <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
         <v>50</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>0.2</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1">
         <v>500</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
       <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
         <v>0.25</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>64</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>98</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>47</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1491,47 +1558,50 @@
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
         <v>200</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>0.2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>2145</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>500</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
       <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
         <v>0.25</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>64</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>90</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>48</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1542,46 +1612,49 @@
         <v>2</v>
       </c>
       <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <v>200</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>0.2</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>2145</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>500</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="4">
         <v>0.01</v>
       </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
         <v>0.15</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>64</v>
       </c>
-      <c r="N16" s="2">
-        <v>11</v>
-      </c>
       <c r="O16" s="2">
+        <v>11</v>
+      </c>
+      <c r="P16" s="2">
         <v>10</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1592,46 +1665,49 @@
         <v>2</v>
       </c>
       <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <v>200</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.2</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>2145</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>500</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0.25</v>
+      <c r="J17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
       </c>
       <c r="M17" s="4">
-        <v>16</v>
-      </c>
-      <c r="N17" s="2">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>64</v>
       </c>
       <c r="O17" s="2">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="P17" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1642,46 +1718,49 @@
         <v>2</v>
       </c>
       <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
         <v>200</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>0.2</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>2145</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>500</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1">
-        <v>64</v>
-      </c>
-      <c r="N18" s="2">
-        <v>90</v>
+      <c r="J18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N18" s="4">
+        <v>16</v>
       </c>
       <c r="O18" s="2">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="P18" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1692,46 +1771,49 @@
         <v>2</v>
       </c>
       <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
         <v>200</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>0.2</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>2145</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>500</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="K19" s="1">
-        <v>0</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0.15</v>
+      <c r="J19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
       </c>
       <c r="M19" s="4">
-        <v>64</v>
-      </c>
-      <c r="N19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N19" s="4">
+        <v>16</v>
+      </c>
+      <c r="O19" s="2">
         <v>100</v>
       </c>
-      <c r="O19" s="2">
-        <v>66</v>
-      </c>
       <c r="P19" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1742,46 +1824,49 @@
         <v>2</v>
       </c>
       <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <v>200</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>0.2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>2145</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>500</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" s="4">
-        <v>0.5</v>
+      <c r="J20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
       </c>
       <c r="M20" s="4">
-        <v>16</v>
-      </c>
-      <c r="N20" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="N20" s="4">
+        <v>64</v>
+      </c>
+      <c r="O20" s="2">
         <v>100</v>
       </c>
-      <c r="O20" s="2">
-        <v>42</v>
-      </c>
       <c r="P20" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1792,46 +1877,49 @@
         <v>2</v>
       </c>
       <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>200</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>0.3</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>2145</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>500</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="1">
         <v>0.01</v>
       </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
       <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
         <v>0.5</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>16</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>100</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2">
         <v>52</v>
       </c>
-      <c r="P21" s="2">
+      <c r="Q21" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1842,46 +1930,49 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
         <v>200</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>0.3</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>2145</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>200</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
       <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
         <v>0.5</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>16</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <v>100</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2">
         <v>56</v>
       </c>
-      <c r="P22" s="2">
+      <c r="Q22" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1892,46 +1983,49 @@
         <v>2</v>
       </c>
       <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
         <v>200</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>0.3</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>2145</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>200</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
       <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <v>0.5</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>64</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>94</v>
       </c>
-      <c r="O23" s="2">
+      <c r="P23" s="2">
         <v>61</v>
       </c>
-      <c r="P23" s="2">
+      <c r="Q23" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1942,46 +2036,49 @@
         <v>2</v>
       </c>
       <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
         <v>200</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>0.3</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>2145</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>200</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
       <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
         <v>0.5</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>128</v>
       </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
         <v>85</v>
       </c>
-      <c r="O24" s="2">
+      <c r="P24" s="2">
         <v>67</v>
       </c>
-      <c r="P24" s="2">
+      <c r="Q24" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1992,46 +2089,49 @@
         <v>2</v>
       </c>
       <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
         <v>200</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>0.3</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>2145</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>200</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
       <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
         <v>0.5</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>256</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
         <v>66</v>
       </c>
-      <c r="O25" s="2">
+      <c r="P25" s="2">
         <v>59</v>
       </c>
-      <c r="P25" s="2">
+      <c r="Q25" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2042,46 +2142,49 @@
         <v>2</v>
       </c>
       <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
         <v>200</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>0.3</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>2145</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>200</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K26" s="1">
-        <v>0</v>
-      </c>
       <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
         <v>0.5</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>32</v>
       </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
         <v>94</v>
       </c>
-      <c r="O26" s="2">
+      <c r="P26" s="2">
         <v>65</v>
       </c>
-      <c r="P26" s="2">
+      <c r="Q26" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2092,46 +2195,49 @@
         <v>2</v>
       </c>
       <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
         <v>200</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>0.3</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>2145</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>200</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="4">
         <v>0.01</v>
       </c>
-      <c r="K27" s="1">
-        <v>0</v>
-      </c>
       <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
         <v>0.5</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>32</v>
       </c>
-      <c r="N27" s="2">
+      <c r="O27" s="2">
         <v>100</v>
       </c>
-      <c r="O27" s="2">
+      <c r="P27" s="2">
         <v>38</v>
       </c>
-      <c r="P27" s="2">
+      <c r="Q27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2142,46 +2248,49 @@
         <v>2</v>
       </c>
       <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
         <v>200</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>0.3</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>2145</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>200</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K28" s="1">
-        <v>0</v>
-      </c>
       <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
         <v>0.5</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>32</v>
       </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
         <v>100</v>
       </c>
-      <c r="O28" s="2">
+      <c r="P28" s="2">
         <v>53</v>
       </c>
-      <c r="P28" s="2">
+      <c r="Q28" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2192,46 +2301,49 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
         <v>200</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>0.3</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>2145</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>200</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="4">
         <v>1E-4</v>
       </c>
-      <c r="K29" s="1">
-        <v>0</v>
-      </c>
       <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
         <v>0.5</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>32</v>
       </c>
-      <c r="N29" s="2">
+      <c r="O29" s="2">
         <v>70</v>
       </c>
-      <c r="O29" s="2">
+      <c r="P29" s="2">
         <v>60</v>
       </c>
-      <c r="P29" s="2">
+      <c r="Q29" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -2242,46 +2354,49 @@
         <v>2</v>
       </c>
       <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
         <v>200</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>0.3</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>2145</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>200</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="1">
         <v>1E-4</v>
       </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="4">
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
         <v>0.2</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>32</v>
-      </c>
-      <c r="N30" s="2">
-        <v>36</v>
       </c>
       <c r="O30" s="2">
         <v>36</v>
       </c>
       <c r="P30" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q30" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -2292,46 +2407,49 @@
         <v>2</v>
       </c>
       <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
         <v>200</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>0.3</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>2145</v>
       </c>
-      <c r="G31" s="4">
+      <c r="H31" s="4">
         <v>1000</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="1">
         <v>1E-4</v>
       </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
       <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
         <v>0.2</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>32</v>
       </c>
-      <c r="N31" s="2">
+      <c r="O31" s="2">
         <v>98</v>
       </c>
-      <c r="O31" s="2">
+      <c r="P31" s="2">
         <v>62</v>
       </c>
-      <c r="P31" s="2">
+      <c r="Q31" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -2342,46 +2460,49 @@
         <v>2</v>
       </c>
       <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
         <v>200</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>0.3</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="4">
         <v>4717</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>1000</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="1">
         <v>1E-4</v>
       </c>
-      <c r="K32" s="1">
-        <v>0</v>
-      </c>
       <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
         <v>0.2</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>32</v>
       </c>
-      <c r="N32" s="2">
+      <c r="O32" s="2">
         <v>93</v>
       </c>
-      <c r="O32" s="2">
+      <c r="P32" s="2">
         <v>32</v>
       </c>
-      <c r="P32" s="2">
+      <c r="Q32" s="2">
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2392,46 +2513,49 @@
         <v>2</v>
       </c>
       <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
         <v>200</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>0.3</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>4717</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>1000</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K33" s="1">
-        <v>0</v>
-      </c>
       <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
         <v>0.2</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>32</v>
       </c>
-      <c r="N33" s="2">
+      <c r="O33" s="2">
         <v>100</v>
       </c>
-      <c r="O33" s="2">
+      <c r="P33" s="2">
         <v>34</v>
       </c>
-      <c r="P33" s="2">
+      <c r="Q33" s="2">
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -2442,414 +2566,659 @@
         <v>2</v>
       </c>
       <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
         <v>200</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>0.3</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>4717</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>1000</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K34" s="1">
-        <v>0</v>
-      </c>
-      <c r="L34" s="4">
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="4">
         <v>0.5</v>
       </c>
-      <c r="M34" s="4">
+      <c r="N34" s="4">
         <v>64</v>
       </c>
-      <c r="N34" s="2">
+      <c r="O34" s="2">
         <v>100</v>
       </c>
-      <c r="O34" s="2">
+      <c r="P34" s="2">
         <v>30</v>
       </c>
-      <c r="P34" s="2">
+      <c r="Q34" s="2">
         <v>270</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
       <c r="B35" s="4">
         <v>10</v>
       </c>
-      <c r="C35" s="6">
-        <v>2</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="6">
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
         <v>0.3</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
         <v>14922</v>
       </c>
-      <c r="G35" s="6">
+      <c r="H35" s="1">
         <v>1000</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="6">
+      <c r="I35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K35" s="6">
-        <v>0</v>
-      </c>
-      <c r="L35" s="6">
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
         <v>0.5</v>
       </c>
-      <c r="M35" s="6">
+      <c r="N35" s="1">
         <v>64</v>
       </c>
-      <c r="N35" s="2">
+      <c r="O35" s="2">
         <v>67</v>
       </c>
-      <c r="O35" s="2">
+      <c r="P35" s="2">
         <v>44</v>
       </c>
-      <c r="P35" s="2">
+      <c r="Q35" s="2">
         <v>967</v>
       </c>
-      <c r="Q35" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="1">
         <v>10</v>
       </c>
-      <c r="C36" s="6">
-        <v>2</v>
-      </c>
-      <c r="D36" s="6">
-        <v>0</v>
-      </c>
-      <c r="E36" s="6">
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
         <v>0.3</v>
       </c>
-      <c r="F36" s="6">
+      <c r="G36" s="1">
         <v>14922</v>
       </c>
-      <c r="G36" s="4">
+      <c r="H36" s="4">
         <v>200</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" s="4">
+      <c r="I36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="4">
         <v>0.01</v>
       </c>
-      <c r="K36" s="6">
-        <v>0</v>
-      </c>
-      <c r="L36" s="6">
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
         <v>0.5</v>
       </c>
-      <c r="M36" s="4">
+      <c r="N36" s="4">
         <v>32</v>
       </c>
-      <c r="N36" s="2">
+      <c r="O36" s="2">
         <v>58</v>
       </c>
-      <c r="O36" s="2">
+      <c r="P36" s="2">
         <v>38</v>
       </c>
-      <c r="P36" s="2">
+      <c r="Q36" s="2">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="1">
         <v>10</v>
       </c>
-      <c r="C37" s="6">
-        <v>2</v>
-      </c>
-      <c r="D37" s="6">
-        <v>0</v>
-      </c>
-      <c r="E37" s="6">
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
         <v>0.3</v>
       </c>
-      <c r="F37" s="6">
+      <c r="G37" s="1">
         <v>14922</v>
       </c>
-      <c r="G37" s="6">
+      <c r="H37" s="1">
         <v>200</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="6">
+      <c r="I37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="1">
         <v>0.01</v>
       </c>
-      <c r="K37" s="6">
-        <v>0</v>
-      </c>
-      <c r="L37" s="4">
-        <v>0</v>
-      </c>
-      <c r="M37" s="6">
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
         <v>32</v>
-      </c>
-      <c r="N37" s="2">
-        <v>30</v>
       </c>
       <c r="O37" s="2">
         <v>30</v>
       </c>
       <c r="P37" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q37" s="2">
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="1">
         <v>10</v>
       </c>
-      <c r="C38" s="6">
-        <v>2</v>
-      </c>
-      <c r="D38" s="6">
-        <v>0</v>
-      </c>
-      <c r="E38" s="6">
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
         <v>0.3</v>
       </c>
-      <c r="F38" s="6">
+      <c r="G38" s="1">
         <v>14922</v>
       </c>
-      <c r="G38" s="6">
+      <c r="H38" s="1">
         <v>200</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="6">
+      <c r="I38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="1">
         <v>0.01</v>
       </c>
-      <c r="K38" s="6">
-        <v>0</v>
-      </c>
-      <c r="L38" s="6">
-        <v>0</v>
-      </c>
-      <c r="M38" s="4">
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4">
         <v>64</v>
       </c>
-      <c r="N38" s="2">
+      <c r="O38" s="2">
         <v>63</v>
       </c>
-      <c r="O38" s="2">
+      <c r="P38" s="2">
         <v>40</v>
       </c>
-      <c r="P38" s="2">
+      <c r="Q38" s="2">
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="1">
         <v>10</v>
       </c>
-      <c r="C39" s="6">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6">
-        <v>0</v>
-      </c>
-      <c r="E39" s="6">
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
         <v>0.3</v>
       </c>
-      <c r="F39" s="6">
+      <c r="G39" s="1">
         <v>14922</v>
       </c>
-      <c r="G39" s="4">
+      <c r="H39" s="4">
         <v>100</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J39" s="6">
+      <c r="I39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="1">
         <v>0.01</v>
       </c>
-      <c r="K39" s="6">
-        <v>0</v>
-      </c>
-      <c r="L39" s="6">
-        <v>0</v>
-      </c>
-      <c r="M39" s="4">
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4">
         <v>128</v>
       </c>
-      <c r="N39" s="2">
+      <c r="O39" s="2">
         <v>56</v>
       </c>
-      <c r="O39" s="2">
+      <c r="P39" s="2">
         <v>41</v>
       </c>
-      <c r="P39" s="2">
+      <c r="Q39" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="1">
         <v>10</v>
       </c>
-      <c r="C40" s="6">
-        <v>2</v>
-      </c>
-      <c r="D40" s="6">
-        <v>0</v>
-      </c>
-      <c r="E40" s="6">
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
         <v>0.3</v>
       </c>
-      <c r="F40" s="6">
+      <c r="G40" s="1">
         <v>14922</v>
       </c>
-      <c r="G40" s="6">
+      <c r="H40" s="1">
         <v>100</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J40" s="4">
+      <c r="I40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="4">
         <v>1E-3</v>
       </c>
-      <c r="K40" s="6">
-        <v>0</v>
-      </c>
-      <c r="L40" s="6">
-        <v>0</v>
-      </c>
-      <c r="M40" s="6">
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1">
         <v>128</v>
       </c>
-      <c r="N40" s="2">
+      <c r="O40" s="2">
         <v>60</v>
       </c>
-      <c r="O40" s="2">
+      <c r="P40" s="2">
         <v>54</v>
       </c>
-      <c r="P40" s="2">
+      <c r="Q40" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="1">
         <v>10</v>
       </c>
-      <c r="C41" s="6">
-        <v>2</v>
-      </c>
-      <c r="D41" s="6">
-        <v>0</v>
-      </c>
-      <c r="E41" s="6">
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
         <v>0.3</v>
       </c>
-      <c r="F41" s="6">
+      <c r="G41" s="1">
         <v>14922</v>
       </c>
-      <c r="G41" s="4">
+      <c r="H41" s="4">
         <v>300</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J41" s="6">
+      <c r="I41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K41" s="6">
-        <v>0</v>
-      </c>
-      <c r="L41" s="6">
-        <v>0</v>
-      </c>
-      <c r="M41" s="6">
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1">
         <v>128</v>
       </c>
-      <c r="N41" s="2">
+      <c r="O41" s="2">
         <v>63</v>
       </c>
-      <c r="O41" s="2">
+      <c r="P41" s="2">
         <v>49</v>
       </c>
-      <c r="P41" s="2">
+      <c r="Q41" s="2">
         <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>38</v>
+      </c>
+      <c r="B42" s="7">
+        <v>10</v>
+      </c>
+      <c r="C42" s="7">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="4">
+        <v>8959</v>
+      </c>
+      <c r="H42" s="4">
+        <v>100</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="L42" s="7">
+        <v>0</v>
+      </c>
+      <c r="M42" s="7">
+        <v>0</v>
+      </c>
+      <c r="N42" s="7">
+        <v>128</v>
+      </c>
+      <c r="O42" s="2">
+        <v>72</v>
+      </c>
+      <c r="P42" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>50</v>
+      </c>
+      <c r="R42" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>39</v>
+      </c>
+      <c r="B43" s="7">
+        <v>10</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3520</v>
+      </c>
+      <c r="H43" s="4">
+        <v>300</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="L43" s="7">
+        <v>0</v>
+      </c>
+      <c r="M43" s="7">
+        <v>0</v>
+      </c>
+      <c r="N43" s="7">
+        <v>128</v>
+      </c>
+      <c r="O43" s="2">
+        <v>96</v>
+      </c>
+      <c r="P43" s="2">
+        <v>56</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>57</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>40</v>
+      </c>
+      <c r="B44" s="7">
+        <v>10</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G44" s="4">
+        <v>22140</v>
+      </c>
+      <c r="H44" s="4">
+        <v>500</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="L44" s="7">
+        <v>0</v>
+      </c>
+      <c r="M44" s="7">
+        <v>0</v>
+      </c>
+      <c r="N44" s="7">
+        <v>128</v>
+      </c>
+      <c r="O44" s="2">
+        <v>81</v>
+      </c>
+      <c r="P44" s="2">
+        <v>66</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>624</v>
+      </c>
+      <c r="R44" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>41</v>
+      </c>
+      <c r="B45" s="7">
+        <v>10</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="7">
+        <v>22140</v>
+      </c>
+      <c r="H45" s="7">
+        <v>500</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="L45" s="7">
+        <v>0</v>
+      </c>
+      <c r="M45" s="7">
+        <v>0</v>
+      </c>
+      <c r="N45" s="4">
+        <v>64</v>
+      </c>
+      <c r="O45" s="2">
+        <v>87</v>
+      </c>
+      <c r="P45" s="2">
+        <v>68</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="B1:N1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
extra training on bigger data sets + memory optimisation
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874E777-DF16-4DFF-90E0-34B3DF70A8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7D9A5-87AC-420E-8F8B-D06E592201C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="41">
   <si>
     <t>test number</t>
   </si>
@@ -169,6 +169,47 @@
   <si>
     <t>filtered by looking at 50-100 files per folder</t>
   </si>
+  <si>
+    <t>best iteration model file path</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>first instance of saving best model to file
+after this, the best testing accuracy is saved
+alongside the corresponding training accuracy</t>
+  </si>
+  <si>
+    <t>top-5 error</t>
+  </si>
+  <si>
+    <t>top 5 error introduced</t>
+  </si>
+  <si>
+    <t>best_model_001.pth</t>
+  </si>
+  <si>
+    <t>best_model_002.pth</t>
+  </si>
+  <si>
+    <t>[100, 150]</t>
+  </si>
+  <si>
+    <t>best_model_003.pth</t>
+  </si>
+  <si>
+    <t>best_model_004.pth</t>
+  </si>
+  <si>
+    <t>best_model_005.pth</t>
+  </si>
+  <si>
+    <t>best_model_006.pth</t>
+  </si>
+  <si>
+    <t>best_model_007.pth</t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,23 +296,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -294,6 +338,41 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -435,6 +514,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -480,30 +562,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:R45" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A2:R45" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T53" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:T53" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S45">
     <sortCondition ref="A2:A45"/>
   </sortState>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="18"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="17"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="5"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 error" dataDxfId="5"/>
     <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -806,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G37" workbookViewId="0">
+      <selection activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,32 +915,35 @@
     <col min="15" max="15" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="41.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -909,10 +996,16 @@
         <v>9</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -964,8 +1057,14 @@
       <c r="Q3" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1017,8 +1116,14 @@
       <c r="Q4" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1070,8 +1175,14 @@
       <c r="Q5" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1123,8 +1234,14 @@
       <c r="Q6" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1176,8 +1293,14 @@
       <c r="Q7" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1229,8 +1352,14 @@
       <c r="Q8" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1282,8 +1411,14 @@
       <c r="Q9" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1335,8 +1470,14 @@
       <c r="Q10" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1388,8 +1529,14 @@
       <c r="Q11" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1441,8 +1588,14 @@
       <c r="Q12" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1494,8 +1647,14 @@
       <c r="Q13" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1547,8 +1706,14 @@
       <c r="Q14" s="2">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1600,8 +1765,14 @@
       <c r="Q15" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1653,8 +1824,14 @@
       <c r="Q16" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1706,8 +1883,14 @@
       <c r="Q17" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1759,8 +1942,14 @@
       <c r="Q18" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1812,8 +2001,14 @@
       <c r="Q19" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1865,8 +2060,14 @@
       <c r="Q20" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1918,8 +2119,14 @@
       <c r="Q21" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1971,8 +2178,14 @@
       <c r="Q22" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2024,8 +2237,14 @@
       <c r="Q23" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2077,8 +2296,14 @@
       <c r="Q24" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2130,8 +2355,14 @@
       <c r="Q25" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2183,8 +2414,14 @@
       <c r="Q26" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2236,8 +2473,14 @@
       <c r="Q27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2289,8 +2532,14 @@
       <c r="Q28" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2342,8 +2591,14 @@
       <c r="Q29" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -2395,8 +2650,14 @@
       <c r="Q30" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -2448,8 +2709,14 @@
       <c r="Q31" s="2">
         <v>126</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -2501,8 +2768,14 @@
       <c r="Q32" s="2">
         <v>297</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2554,8 +2827,14 @@
       <c r="Q33" s="2">
         <v>297</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -2607,8 +2886,14 @@
       <c r="Q34" s="2">
         <v>270</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="R34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -2660,11 +2945,17 @@
       <c r="Q35" s="2">
         <v>967</v>
       </c>
-      <c r="R35" s="5" t="s">
+      <c r="R35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S35" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T35" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -2716,8 +3007,14 @@
       <c r="Q36" s="2">
         <v>252</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -2769,8 +3066,14 @@
       <c r="Q37" s="2">
         <v>242</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -2822,8 +3125,14 @@
       <c r="Q38" s="2">
         <v>185</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -2875,8 +3184,14 @@
       <c r="Q39" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -2928,8 +3243,14 @@
       <c r="Q40" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -2981,24 +3302,30 @@
       <c r="Q41" s="2">
         <v>190</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="1">
         <v>10</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="1">
         <v>2</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="7">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7">
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
         <v>0.3</v>
       </c>
       <c r="G42" s="4">
@@ -3007,22 +3334,22 @@
       <c r="H42" s="4">
         <v>100</v>
       </c>
-      <c r="I42" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K42" s="7">
+      <c r="I42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L42" s="7">
-        <v>0</v>
-      </c>
-      <c r="M42" s="7">
-        <v>0</v>
-      </c>
-      <c r="N42" s="7">
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
         <v>128</v>
       </c>
       <c r="O42" s="2">
@@ -3034,27 +3361,33 @@
       <c r="Q42" s="2">
         <v>50</v>
       </c>
-      <c r="R42" s="8" t="s">
+      <c r="R42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S42" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="T42" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="1">
         <v>10</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="1">
         <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="7">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7">
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
         <v>0.3</v>
       </c>
       <c r="G43" s="4">
@@ -3063,22 +3396,22 @@
       <c r="H43" s="4">
         <v>300</v>
       </c>
-      <c r="I43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K43" s="7">
+      <c r="I43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L43" s="7">
-        <v>0</v>
-      </c>
-      <c r="M43" s="7">
-        <v>0</v>
-      </c>
-      <c r="N43" s="7">
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
         <v>128</v>
       </c>
       <c r="O43" s="2">
@@ -3090,27 +3423,33 @@
       <c r="Q43" s="2">
         <v>57</v>
       </c>
-      <c r="R43" s="8" t="s">
+      <c r="R43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S43" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="T43" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="1">
         <v>10</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="1">
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="7">
-        <v>0</v>
-      </c>
-      <c r="F44" s="7">
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
         <v>0.3</v>
       </c>
       <c r="G44" s="4">
@@ -3119,22 +3458,22 @@
       <c r="H44" s="4">
         <v>500</v>
       </c>
-      <c r="I44" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44" s="7">
+      <c r="I44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L44" s="7">
-        <v>0</v>
-      </c>
-      <c r="M44" s="7">
-        <v>0</v>
-      </c>
-      <c r="N44" s="7">
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1">
         <v>128</v>
       </c>
       <c r="O44" s="2">
@@ -3146,48 +3485,54 @@
       <c r="Q44" s="2">
         <v>624</v>
       </c>
-      <c r="R44" s="8" t="s">
+      <c r="R44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S44" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T44" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="1">
         <v>10</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="1">
         <v>2</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="7">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7">
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
         <v>0.3</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="1">
         <v>22140</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="1">
         <v>500</v>
       </c>
-      <c r="I45" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K45" s="7">
+      <c r="I45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L45" s="7">
-        <v>0</v>
-      </c>
-      <c r="M45" s="7">
+      <c r="L45" s="1">
+        <v>0</v>
+      </c>
+      <c r="M45" s="1">
         <v>0</v>
       </c>
       <c r="N45" s="4">
@@ -3201,6 +3546,490 @@
       </c>
       <c r="Q45" s="2">
         <v>630</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1">
+        <v>10</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G46" s="4">
+        <v>18480</v>
+      </c>
+      <c r="H46" s="1">
+        <v>500</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0</v>
+      </c>
+      <c r="N46" s="4">
+        <v>64</v>
+      </c>
+      <c r="O46" s="2">
+        <v>84</v>
+      </c>
+      <c r="P46" s="2">
+        <v>67</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>515</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="4">
+        <v>13560</v>
+      </c>
+      <c r="H47" s="1">
+        <v>500</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1">
+        <v>64</v>
+      </c>
+      <c r="O47" s="2">
+        <v>83</v>
+      </c>
+      <c r="P47" s="2">
+        <v>59</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>523</v>
+      </c>
+      <c r="R47" s="8">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="S47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44</v>
+      </c>
+      <c r="B48" s="10">
+        <v>10</v>
+      </c>
+      <c r="C48" s="10">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G48" s="4">
+        <v>22140</v>
+      </c>
+      <c r="H48" s="4">
+        <v>100</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L48" s="10">
+        <v>0</v>
+      </c>
+      <c r="M48" s="10">
+        <v>0</v>
+      </c>
+      <c r="N48" s="10">
+        <v>64</v>
+      </c>
+      <c r="O48" s="2">
+        <v>83</v>
+      </c>
+      <c r="P48" s="2">
+        <v>70</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>140</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>45</v>
+      </c>
+      <c r="B49" s="4">
+        <v>25</v>
+      </c>
+      <c r="C49" s="10">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="10">
+        <v>0</v>
+      </c>
+      <c r="F49" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G49" s="4">
+        <v>70675</v>
+      </c>
+      <c r="H49" s="10">
+        <v>100</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K49" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L49" s="10">
+        <v>0</v>
+      </c>
+      <c r="M49" s="10">
+        <v>0</v>
+      </c>
+      <c r="N49" s="10">
+        <v>64</v>
+      </c>
+      <c r="O49" s="2">
+        <v>60</v>
+      </c>
+      <c r="P49" s="2">
+        <v>51</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>393</v>
+      </c>
+      <c r="R49" s="8">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>46</v>
+      </c>
+      <c r="B50" s="10">
+        <v>25</v>
+      </c>
+      <c r="C50" s="10">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="10">
+        <v>0</v>
+      </c>
+      <c r="F50" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G50" s="4">
+        <v>69250</v>
+      </c>
+      <c r="H50" s="10">
+        <v>100</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L50" s="10">
+        <v>0</v>
+      </c>
+      <c r="M50" s="10">
+        <v>0</v>
+      </c>
+      <c r="N50" s="10">
+        <v>64</v>
+      </c>
+      <c r="O50" s="2">
+        <v>43</v>
+      </c>
+      <c r="P50" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>389</v>
+      </c>
+      <c r="R50" s="8">
+        <v>0.68720000000000003</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>47</v>
+      </c>
+      <c r="B51" s="10">
+        <v>25</v>
+      </c>
+      <c r="C51" s="10">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="10">
+        <v>0</v>
+      </c>
+      <c r="F51" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G51" s="10">
+        <v>69250</v>
+      </c>
+      <c r="H51" s="10">
+        <v>100</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="L51" s="10">
+        <v>0</v>
+      </c>
+      <c r="M51" s="10">
+        <v>0</v>
+      </c>
+      <c r="N51" s="10">
+        <v>64</v>
+      </c>
+      <c r="O51" s="2">
+        <v>48</v>
+      </c>
+      <c r="P51" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>393</v>
+      </c>
+      <c r="R51" s="8">
+        <v>0.76029999999999998</v>
+      </c>
+      <c r="T51" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>48</v>
+      </c>
+      <c r="B52" s="10">
+        <v>25</v>
+      </c>
+      <c r="C52" s="10">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="10">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G52" s="10">
+        <v>69250</v>
+      </c>
+      <c r="H52" s="10">
+        <v>100</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="L52" s="10">
+        <v>0</v>
+      </c>
+      <c r="M52" s="10">
+        <v>0</v>
+      </c>
+      <c r="N52" s="4">
+        <v>32</v>
+      </c>
+      <c r="O52" s="2">
+        <v>38</v>
+      </c>
+      <c r="P52" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>400</v>
+      </c>
+      <c r="R52" s="8">
+        <v>0.6452</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>49</v>
+      </c>
+      <c r="B53" s="10">
+        <v>25</v>
+      </c>
+      <c r="C53" s="10">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="10">
+        <v>0</v>
+      </c>
+      <c r="F53" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G53" s="10">
+        <v>69250</v>
+      </c>
+      <c r="H53" s="10">
+        <v>100</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="L53" s="10">
+        <v>0</v>
+      </c>
+      <c r="M53" s="10">
+        <v>0</v>
+      </c>
+      <c r="N53" s="4">
+        <v>128</v>
+      </c>
+      <c r="O53" s="2">
+        <v>38</v>
+      </c>
+      <c r="P53" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>721</v>
+      </c>
+      <c r="R53" s="8">
+        <v>0.72209999999999996</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3210,15 +4039,15 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
further audio tests, included proportions of accuracy/splits, + adamw optimizer
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7D9A5-87AC-420E-8F8B-D06E592201C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529CE36E-B45F-4EC2-9488-77BD3C5FB60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="50">
   <si>
     <t>test number</t>
   </si>
@@ -209,6 +209,37 @@
   </si>
   <si>
     <t>best_model_007.pth</t>
+  </si>
+  <si>
+    <t>best_model_008.pth</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>best_model_009.pth</t>
+  </si>
+  <si>
+    <t>best_model_010.pth</t>
+  </si>
+  <si>
+    <t>first switch to adam optimizer.
+DOES use more memory than SGD but
+provides better results</t>
+  </si>
+  <si>
+    <t>AdamW</t>
+  </si>
+  <si>
+    <t>usage of adamW due to convergence and
+separating of weight decay and parameter
+updates</t>
+  </si>
+  <si>
+    <t>best_model_011.pth</t>
+  </si>
+  <si>
+    <t>best_model_012.pth</t>
   </si>
 </sst>
 </file>
@@ -562,8 +593,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T53" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A2:T53" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T58" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:T58" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S45">
     <sortCondition ref="A2:A45"/>
   </sortState>
@@ -890,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G37" workbookViewId="0">
-      <selection activeCell="R54" sqref="R54"/>
+    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
+      <selection activeCell="R59" sqref="R59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,19 +3713,19 @@
       <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="1">
         <v>10</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="1">
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="10">
-        <v>0</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
         <v>0.3</v>
       </c>
       <c r="G48" s="4">
@@ -3703,22 +3734,22 @@
       <c r="H48" s="4">
         <v>100</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K48" s="10">
+      <c r="I48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L48" s="10">
-        <v>0</v>
-      </c>
-      <c r="M48" s="10">
-        <v>0</v>
-      </c>
-      <c r="N48" s="10">
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1">
+        <v>0</v>
+      </c>
+      <c r="N48" s="1">
         <v>64</v>
       </c>
       <c r="O48" s="2">
@@ -3744,40 +3775,40 @@
       <c r="B49" s="4">
         <v>25</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="1">
         <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="10">
-        <v>0</v>
-      </c>
-      <c r="F49" s="10">
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
         <v>0.3</v>
       </c>
       <c r="G49" s="4">
         <v>70675</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H49" s="1">
         <v>100</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K49" s="10">
+      <c r="I49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K49" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L49" s="10">
-        <v>0</v>
-      </c>
-      <c r="M49" s="10">
-        <v>0</v>
-      </c>
-      <c r="N49" s="10">
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0</v>
+      </c>
+      <c r="N49" s="1">
         <v>64</v>
       </c>
       <c r="O49" s="2">
@@ -3800,43 +3831,43 @@
       <c r="A50" s="1">
         <v>46</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="1">
         <v>25</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="1">
         <v>2</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="10">
-        <v>0</v>
-      </c>
-      <c r="F50" s="10">
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
         <v>0.3</v>
       </c>
       <c r="G50" s="4">
         <v>69250</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H50" s="1">
         <v>100</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K50" s="10">
+      <c r="I50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L50" s="10">
-        <v>0</v>
-      </c>
-      <c r="M50" s="10">
-        <v>0</v>
-      </c>
-      <c r="N50" s="10">
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
+      <c r="N50" s="1">
         <v>64</v>
       </c>
       <c r="O50" s="2">
@@ -3859,43 +3890,43 @@
       <c r="A51" s="1">
         <v>47</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="1">
         <v>25</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="1">
         <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E51" s="10">
-        <v>0</v>
-      </c>
-      <c r="F51" s="10">
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
         <v>0.3</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="1">
         <v>69250</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="1">
         <v>100</v>
       </c>
-      <c r="I51" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J51" s="10" t="s">
+      <c r="I51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K51" s="4">
         <v>0.01</v>
       </c>
-      <c r="L51" s="10">
-        <v>0</v>
-      </c>
-      <c r="M51" s="10">
-        <v>0</v>
-      </c>
-      <c r="N51" s="10">
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0</v>
+      </c>
+      <c r="N51" s="1">
         <v>64</v>
       </c>
       <c r="O51" s="2">
@@ -3918,40 +3949,40 @@
       <c r="A52" s="1">
         <v>48</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="1">
         <v>25</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="1">
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E52" s="10">
-        <v>0</v>
-      </c>
-      <c r="F52" s="10">
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
         <v>0.3</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="1">
         <v>69250</v>
       </c>
-      <c r="H52" s="10">
+      <c r="H52" s="1">
         <v>100</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K52" s="10">
+      <c r="I52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="1">
         <v>0.01</v>
       </c>
-      <c r="L52" s="10">
-        <v>0</v>
-      </c>
-      <c r="M52" s="10">
+      <c r="L52" s="1">
+        <v>0</v>
+      </c>
+      <c r="M52" s="1">
         <v>0</v>
       </c>
       <c r="N52" s="4">
@@ -3977,40 +4008,40 @@
       <c r="A53" s="1">
         <v>49</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="1">
         <v>25</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="1">
         <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="10">
-        <v>0</v>
-      </c>
-      <c r="F53" s="10">
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
         <v>0.3</v>
       </c>
-      <c r="G53" s="10">
+      <c r="G53" s="1">
         <v>69250</v>
       </c>
-      <c r="H53" s="10">
+      <c r="H53" s="1">
         <v>100</v>
       </c>
-      <c r="I53" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J53" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K53" s="10">
+      <c r="I53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="1">
         <v>0.01</v>
       </c>
-      <c r="L53" s="10">
-        <v>0</v>
-      </c>
-      <c r="M53" s="10">
+      <c r="L53" s="1">
+        <v>0</v>
+      </c>
+      <c r="M53" s="1">
         <v>0</v>
       </c>
       <c r="N53" s="4">
@@ -4030,6 +4061,305 @@
       </c>
       <c r="T53" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G54" s="4">
+        <v>70325</v>
+      </c>
+      <c r="H54" s="1">
+        <v>100</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K54" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+      <c r="M54" s="1">
+        <v>0</v>
+      </c>
+      <c r="N54" s="4">
+        <v>16</v>
+      </c>
+      <c r="O54" s="2">
+        <v>39</v>
+      </c>
+      <c r="P54" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>546</v>
+      </c>
+      <c r="R54" s="8">
+        <v>0.7097</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>51</v>
+      </c>
+      <c r="B55" s="10">
+        <v>25</v>
+      </c>
+      <c r="C55" s="10">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="10">
+        <v>0</v>
+      </c>
+      <c r="F55" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G55" s="10">
+        <v>70325</v>
+      </c>
+      <c r="H55" s="10">
+        <v>100</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="L55" s="10">
+        <v>0</v>
+      </c>
+      <c r="M55" s="10">
+        <v>0</v>
+      </c>
+      <c r="N55" s="10">
+        <v>16</v>
+      </c>
+      <c r="O55" s="2">
+        <v>48</v>
+      </c>
+      <c r="P55" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>541</v>
+      </c>
+      <c r="R55" s="8">
+        <v>0.73860000000000003</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>52</v>
+      </c>
+      <c r="B56" s="10">
+        <v>25</v>
+      </c>
+      <c r="C56" s="10">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="10">
+        <v>0</v>
+      </c>
+      <c r="F56" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G56" s="10">
+        <v>70325</v>
+      </c>
+      <c r="H56" s="10">
+        <v>100</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K56" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L56" s="10">
+        <v>0</v>
+      </c>
+      <c r="M56" s="10">
+        <v>0</v>
+      </c>
+      <c r="N56" s="10">
+        <v>16</v>
+      </c>
+      <c r="O56" s="2">
+        <v>47</v>
+      </c>
+      <c r="P56" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>1050</v>
+      </c>
+      <c r="R56" s="8">
+        <v>0.76690000000000003</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>53</v>
+      </c>
+      <c r="B57" s="10">
+        <v>25</v>
+      </c>
+      <c r="C57" s="10">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="10">
+        <v>0</v>
+      </c>
+      <c r="F57" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G57" s="10">
+        <v>70325</v>
+      </c>
+      <c r="H57" s="10">
+        <v>100</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K57" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L57" s="10">
+        <v>0</v>
+      </c>
+      <c r="M57" s="10">
+        <v>0</v>
+      </c>
+      <c r="N57" s="10">
+        <v>16</v>
+      </c>
+      <c r="O57" s="2">
+        <v>42</v>
+      </c>
+      <c r="P57" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>592</v>
+      </c>
+      <c r="R57" s="8">
+        <v>0.71640000000000004</v>
+      </c>
+      <c r="S57" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>54</v>
+      </c>
+      <c r="B58" s="10">
+        <v>25</v>
+      </c>
+      <c r="C58" s="10">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="10">
+        <v>0</v>
+      </c>
+      <c r="F58" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="10">
+        <v>100</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K58" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L58" s="10">
+        <v>0</v>
+      </c>
+      <c r="M58" s="10">
+        <v>0</v>
+      </c>
+      <c r="N58" s="10">
+        <v>16</v>
+      </c>
+      <c r="O58" s="2">
+        <v>53</v>
+      </c>
+      <c r="P58" s="2">
+        <v>47</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>604</v>
+      </c>
+      <c r="R58" s="8">
+        <v>0.78759999999999997</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some supercomputer cnn test results
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529CE36E-B45F-4EC2-9488-77BD3C5FB60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E0A82-C41E-4693-9901-F61EB774834D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
   <si>
     <t>test number</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>best_model_012.pth</t>
+  </si>
+  <si>
+    <t>first ever test using SCIAMA.</t>
+  </si>
+  <si>
+    <t>[0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 50]</t>
   </si>
 </sst>
 </file>
@@ -593,8 +602,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T58" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A2:T58" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T64" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:T64" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S45">
     <sortCondition ref="A2:A45"/>
   </sortState>
@@ -921,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4126,43 +4135,43 @@
       <c r="A55" s="1">
         <v>51</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="1">
         <v>25</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="1">
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E55" s="10">
-        <v>0</v>
-      </c>
-      <c r="F55" s="10">
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
         <v>0.3</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G55" s="1">
         <v>70325</v>
       </c>
-      <c r="H55" s="10">
+      <c r="H55" s="1">
         <v>100</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="10" t="s">
+      <c r="I55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K55" s="4">
         <v>1E-3</v>
       </c>
-      <c r="L55" s="10">
-        <v>0</v>
-      </c>
-      <c r="M55" s="10">
-        <v>0</v>
-      </c>
-      <c r="N55" s="10">
+      <c r="L55" s="1">
+        <v>0</v>
+      </c>
+      <c r="M55" s="1">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1">
         <v>16</v>
       </c>
       <c r="O55" s="2">
@@ -4185,43 +4194,43 @@
       <c r="A56" s="1">
         <v>52</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="1">
         <v>25</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="1">
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E56" s="10">
-        <v>0</v>
-      </c>
-      <c r="F56" s="10">
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
         <v>0.3</v>
       </c>
-      <c r="G56" s="10">
+      <c r="G56" s="1">
         <v>70325</v>
       </c>
-      <c r="H56" s="10">
+      <c r="H56" s="1">
         <v>100</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="I56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K56" s="10">
+      <c r="K56" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L56" s="10">
-        <v>0</v>
-      </c>
-      <c r="M56" s="10">
-        <v>0</v>
-      </c>
-      <c r="N56" s="10">
+      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+      <c r="M56" s="1">
+        <v>0</v>
+      </c>
+      <c r="N56" s="1">
         <v>16</v>
       </c>
       <c r="O56" s="2">
@@ -4247,43 +4256,43 @@
       <c r="A57" s="1">
         <v>53</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="1">
         <v>25</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="1">
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E57" s="10">
-        <v>0</v>
-      </c>
-      <c r="F57" s="10">
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
         <v>0.3</v>
       </c>
-      <c r="G57" s="10">
+      <c r="G57" s="1">
         <v>70325</v>
       </c>
-      <c r="H57" s="10">
+      <c r="H57" s="1">
         <v>100</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="I57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K57" s="10">
+      <c r="K57" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L57" s="10">
-        <v>0</v>
-      </c>
-      <c r="M57" s="10">
-        <v>0</v>
-      </c>
-      <c r="N57" s="10">
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="M57" s="1">
+        <v>0</v>
+      </c>
+      <c r="N57" s="1">
         <v>16</v>
       </c>
       <c r="O57" s="2">
@@ -4309,41 +4318,43 @@
       <c r="A58" s="1">
         <v>54</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="1">
         <v>25</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="1">
         <v>2</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="10">
-        <v>0</v>
-      </c>
-      <c r="F58" s="10">
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
         <v>0.3</v>
       </c>
-      <c r="G58" s="4"/>
-      <c r="H58" s="10">
+      <c r="G58" s="4">
+        <v>70725</v>
+      </c>
+      <c r="H58" s="1">
         <v>100</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J58" s="4" t="s">
+      <c r="I58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K58" s="10">
+      <c r="K58" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L58" s="10">
-        <v>0</v>
-      </c>
-      <c r="M58" s="10">
-        <v>0</v>
-      </c>
-      <c r="N58" s="10">
+      <c r="L58" s="1">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1">
+        <v>0</v>
+      </c>
+      <c r="N58" s="1">
         <v>16</v>
       </c>
       <c r="O58" s="2">
@@ -4361,6 +4372,343 @@
       <c r="T58" s="2" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="59" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>55</v>
+      </c>
+      <c r="B59" s="4">
+        <v>10</v>
+      </c>
+      <c r="C59" s="10">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="10">
+        <v>0</v>
+      </c>
+      <c r="F59" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G59" s="4">
+        <v>7300</v>
+      </c>
+      <c r="H59" s="10">
+        <v>100</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K59" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L59" s="10">
+        <v>0</v>
+      </c>
+      <c r="M59" s="10">
+        <v>0</v>
+      </c>
+      <c r="N59" s="10">
+        <v>16</v>
+      </c>
+      <c r="O59" s="2">
+        <v>84</v>
+      </c>
+      <c r="P59" s="2">
+        <v>52</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>45</v>
+      </c>
+      <c r="R59" s="8">
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="S59" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T59" s="2"/>
+    </row>
+    <row r="60" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>56</v>
+      </c>
+      <c r="B60" s="10">
+        <v>10</v>
+      </c>
+      <c r="C60" s="10">
+        <v>2</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="10">
+        <v>0</v>
+      </c>
+      <c r="F60" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G60" s="4">
+        <v>10090</v>
+      </c>
+      <c r="H60" s="10">
+        <v>100</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K60" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L60" s="10">
+        <v>0</v>
+      </c>
+      <c r="M60" s="10">
+        <v>0</v>
+      </c>
+      <c r="N60" s="10">
+        <v>16</v>
+      </c>
+      <c r="O60" s="2">
+        <v>96</v>
+      </c>
+      <c r="P60" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>61</v>
+      </c>
+      <c r="R60" s="8">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="T60" s="2"/>
+    </row>
+    <row r="61" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>57</v>
+      </c>
+      <c r="B61" s="10">
+        <v>10</v>
+      </c>
+      <c r="C61" s="10">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="10">
+        <v>0</v>
+      </c>
+      <c r="F61" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G61" s="10">
+        <v>10090</v>
+      </c>
+      <c r="H61" s="10">
+        <v>100</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K61" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L61" s="10">
+        <v>0</v>
+      </c>
+      <c r="M61" s="10">
+        <v>0</v>
+      </c>
+      <c r="N61" s="4">
+        <v>128</v>
+      </c>
+      <c r="O61" s="2">
+        <v>98</v>
+      </c>
+      <c r="P61" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>13</v>
+      </c>
+      <c r="R61" s="8">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="T61" s="2"/>
+    </row>
+    <row r="62" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>58</v>
+      </c>
+      <c r="B62" s="10">
+        <v>10</v>
+      </c>
+      <c r="C62" s="10">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="10">
+        <v>0</v>
+      </c>
+      <c r="F62" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G62" s="10">
+        <v>10090</v>
+      </c>
+      <c r="H62" s="4">
+        <v>500</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K62" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L62" s="10">
+        <v>0</v>
+      </c>
+      <c r="M62" s="10">
+        <v>0</v>
+      </c>
+      <c r="N62" s="4">
+        <v>-1</v>
+      </c>
+      <c r="O62" s="2">
+        <v>93</v>
+      </c>
+      <c r="P62" s="2">
+        <v>76</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>48</v>
+      </c>
+      <c r="R62" s="8">
+        <v>0.97460000000000002</v>
+      </c>
+      <c r="T62" s="2"/>
+    </row>
+    <row r="63" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>59</v>
+      </c>
+      <c r="B63" s="4">
+        <v>25</v>
+      </c>
+      <c r="C63" s="10">
+        <v>2</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="10">
+        <v>0</v>
+      </c>
+      <c r="F63" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G63" s="4">
+        <v>8875</v>
+      </c>
+      <c r="H63" s="10">
+        <v>500</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K63" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L63" s="10">
+        <v>0</v>
+      </c>
+      <c r="M63" s="10">
+        <v>0</v>
+      </c>
+      <c r="N63" s="4">
+        <v>64</v>
+      </c>
+      <c r="O63" s="2">
+        <v>99</v>
+      </c>
+      <c r="P63" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>88</v>
+      </c>
+      <c r="R63" s="8">
+        <v>0.89070000000000005</v>
+      </c>
+      <c r="T63" s="2"/>
+    </row>
+    <row r="64" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>60</v>
+      </c>
+      <c r="B64" s="4">
+        <v>100</v>
+      </c>
+      <c r="C64" s="10">
+        <v>2</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="10">
+        <v>0</v>
+      </c>
+      <c r="F64" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G64" s="4">
+        <v>81600</v>
+      </c>
+      <c r="H64" s="10">
+        <v>500</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K64" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L64" s="10">
+        <v>0</v>
+      </c>
+      <c r="M64" s="10">
+        <v>0</v>
+      </c>
+      <c r="N64" s="4">
+        <v>64</v>
+      </c>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+      <c r="T64" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated code for torchaudio.
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E0A82-C41E-4693-9901-F61EB774834D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BE4BF2-2EA8-4DB3-8EAB-A8D0090DC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="55">
   <si>
     <t>test number</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>[1, 50]</t>
+  </si>
+  <si>
+    <t>used TorchAudio instead of Librosa to load</t>
+  </si>
+  <si>
+    <t>best_model_013.pth</t>
   </si>
 </sst>
 </file>
@@ -932,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="R65" sqref="R65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4342,7 +4348,7 @@
       <c r="I58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J58" s="10" t="s">
+      <c r="J58" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K58" s="1">
@@ -4380,40 +4386,40 @@
       <c r="B59" s="4">
         <v>10</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="1">
         <v>2</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="10">
-        <v>0</v>
-      </c>
-      <c r="F59" s="10">
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
         <v>0.3</v>
       </c>
       <c r="G59" s="4">
         <v>7300</v>
       </c>
-      <c r="H59" s="10">
+      <c r="H59" s="1">
         <v>100</v>
       </c>
-      <c r="I59" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J59" s="10" t="s">
+      <c r="I59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K59" s="10">
+      <c r="K59" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L59" s="10">
-        <v>0</v>
-      </c>
-      <c r="M59" s="10">
-        <v>0</v>
-      </c>
-      <c r="N59" s="10">
+      <c r="L59" s="1">
+        <v>0</v>
+      </c>
+      <c r="M59" s="1">
+        <v>0</v>
+      </c>
+      <c r="N59" s="1">
         <v>16</v>
       </c>
       <c r="O59" s="2">
@@ -4437,43 +4443,43 @@
       <c r="A60" s="1">
         <v>56</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="1">
         <v>10</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="1">
         <v>2</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E60" s="10">
-        <v>0</v>
-      </c>
-      <c r="F60" s="10">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
         <v>0.3</v>
       </c>
       <c r="G60" s="4">
         <v>10090</v>
       </c>
-      <c r="H60" s="10">
+      <c r="H60" s="1">
         <v>100</v>
       </c>
-      <c r="I60" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J60" s="10" t="s">
+      <c r="I60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K60" s="10">
+      <c r="K60" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L60" s="10">
-        <v>0</v>
-      </c>
-      <c r="M60" s="10">
-        <v>0</v>
-      </c>
-      <c r="N60" s="10">
+      <c r="L60" s="1">
+        <v>0</v>
+      </c>
+      <c r="M60" s="1">
+        <v>0</v>
+      </c>
+      <c r="N60" s="1">
         <v>16</v>
       </c>
       <c r="O60" s="2">
@@ -4494,40 +4500,40 @@
       <c r="A61" s="1">
         <v>57</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="1">
         <v>10</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="1">
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E61" s="10">
-        <v>0</v>
-      </c>
-      <c r="F61" s="10">
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
         <v>0.3</v>
       </c>
-      <c r="G61" s="10">
+      <c r="G61" s="1">
         <v>10090</v>
       </c>
-      <c r="H61" s="10">
+      <c r="H61" s="1">
         <v>100</v>
       </c>
-      <c r="I61" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J61" s="10" t="s">
+      <c r="I61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J61" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K61" s="10">
+      <c r="K61" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L61" s="10">
-        <v>0</v>
-      </c>
-      <c r="M61" s="10">
+      <c r="L61" s="1">
+        <v>0</v>
+      </c>
+      <c r="M61" s="1">
         <v>0</v>
       </c>
       <c r="N61" s="4">
@@ -4551,40 +4557,40 @@
       <c r="A62" s="1">
         <v>58</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="1">
         <v>10</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="1">
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E62" s="10">
-        <v>0</v>
-      </c>
-      <c r="F62" s="10">
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
         <v>0.3</v>
       </c>
-      <c r="G62" s="10">
+      <c r="G62" s="1">
         <v>10090</v>
       </c>
       <c r="H62" s="4">
         <v>500</v>
       </c>
-      <c r="I62" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J62" s="10" t="s">
+      <c r="I62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K62" s="10">
+      <c r="K62" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L62" s="10">
-        <v>0</v>
-      </c>
-      <c r="M62" s="10">
+      <c r="L62" s="1">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1">
         <v>0</v>
       </c>
       <c r="N62" s="4">
@@ -4611,37 +4617,37 @@
       <c r="B63" s="4">
         <v>25</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="1">
         <v>2</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E63" s="10">
-        <v>0</v>
-      </c>
-      <c r="F63" s="10">
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
         <v>0.3</v>
       </c>
       <c r="G63" s="4">
         <v>8875</v>
       </c>
-      <c r="H63" s="10">
+      <c r="H63" s="1">
         <v>500</v>
       </c>
-      <c r="I63" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J63" s="10" t="s">
+      <c r="I63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K63" s="10">
+      <c r="K63" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L63" s="10">
-        <v>0</v>
-      </c>
-      <c r="M63" s="10">
+      <c r="L63" s="1">
+        <v>0</v>
+      </c>
+      <c r="M63" s="1">
         <v>0</v>
       </c>
       <c r="N63" s="4">
@@ -4666,13 +4672,13 @@
         <v>60</v>
       </c>
       <c r="B64" s="4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C64" s="10">
         <v>2</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>52</v>
+      <c r="D64" s="4">
+        <v>20</v>
       </c>
       <c r="E64" s="10">
         <v>0</v>
@@ -4681,10 +4687,10 @@
         <v>0.3</v>
       </c>
       <c r="G64" s="4">
-        <v>81600</v>
-      </c>
-      <c r="H64" s="10">
-        <v>500</v>
+        <v>2713</v>
+      </c>
+      <c r="H64" s="4">
+        <v>100</v>
       </c>
       <c r="I64" s="10" t="s">
         <v>12</v>
@@ -4702,13 +4708,26 @@
         <v>0</v>
       </c>
       <c r="N64" s="4">
-        <v>64</v>
-      </c>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
-      <c r="T64" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="O64" s="2">
+        <v>94</v>
+      </c>
+      <c r="P64" s="2">
+        <v>67</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>104</v>
+      </c>
+      <c r="R64" s="8">
+        <v>0.93379999999999996</v>
+      </c>
+      <c r="S64" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="T64" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
running larger scale models on 5060
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BE4BF2-2EA8-4DB3-8EAB-A8D0090DC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66039F5A-9EDD-4C50-9445-066850CB4A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="61">
   <si>
     <t>test number</t>
   </si>
@@ -181,9 +181,6 @@
 alongside the corresponding training accuracy</t>
   </si>
   <si>
-    <t>top-5 error</t>
-  </si>
-  <si>
     <t>top 5 error introduced</t>
   </si>
   <si>
@@ -255,6 +252,27 @@
   </si>
   <si>
     <t>best_model_013.pth</t>
+  </si>
+  <si>
+    <t>best_model_014.pth</t>
+  </si>
+  <si>
+    <t>best_model_015.pth</t>
+  </si>
+  <si>
+    <t>top-5 accuracy</t>
+  </si>
+  <si>
+    <t>best_model_016.pth</t>
+  </si>
+  <si>
+    <t>best_model_017.pth</t>
+  </si>
+  <si>
+    <t>best_model_018.pth</t>
+  </si>
+  <si>
+    <t>best_model_019.pth</t>
   </si>
 </sst>
 </file>
@@ -608,8 +626,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T64" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A2:T64" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T70" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:T70" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S45">
     <sortCondition ref="A2:A45"/>
   </sortState>
@@ -631,7 +649,7 @@
     <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="8"/>
     <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="7"/>
     <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 error" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="5"/>
     <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
     <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="3"/>
   </tableColumns>
@@ -936,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView tabSelected="1" topLeftCell="G51" workbookViewId="0">
+      <selection activeCell="T71" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>6</v>
@@ -3659,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3718,10 +3736,10 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3839,7 +3857,7 @@
         <v>0.81869999999999998</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3853,7 +3871,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -3898,7 +3916,7 @@
         <v>0.68720000000000003</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3912,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -3957,7 +3975,7 @@
         <v>0.76029999999999998</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3971,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -4016,7 +4034,7 @@
         <v>0.6452</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4030,7 +4048,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -4075,7 +4093,7 @@
         <v>0.72209999999999996</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4089,7 +4107,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -4134,7 +4152,7 @@
         <v>0.7097</v>
       </c>
       <c r="T54" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4148,7 +4166,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -4193,7 +4211,7 @@
         <v>0.73860000000000003</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="45" x14ac:dyDescent="0.25">
@@ -4207,7 +4225,7 @@
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -4225,7 +4243,7 @@
         <v>12</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K56" s="1">
         <v>1E-3</v>
@@ -4252,10 +4270,10 @@
         <v>0.76690000000000003</v>
       </c>
       <c r="S56" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T56" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="45" x14ac:dyDescent="0.25">
@@ -4269,7 +4287,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -4287,7 +4305,7 @@
         <v>12</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K57" s="1">
         <v>1E-3</v>
@@ -4314,10 +4332,10 @@
         <v>0.71640000000000004</v>
       </c>
       <c r="S57" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T57" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4349,7 +4367,7 @@
         <v>12</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K58" s="1">
         <v>1E-3</v>
@@ -4376,7 +4394,7 @@
         <v>0.78759999999999997</v>
       </c>
       <c r="T58" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4408,7 +4426,7 @@
         <v>12</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K59" s="1">
         <v>1E-3</v>
@@ -4435,7 +4453,7 @@
         <v>0.87439999999999996</v>
       </c>
       <c r="S59" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T59" s="2"/>
     </row>
@@ -4450,7 +4468,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -4468,7 +4486,7 @@
         <v>12</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K60" s="1">
         <v>1E-3</v>
@@ -4507,7 +4525,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -4525,7 +4543,7 @@
         <v>12</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K61" s="1">
         <v>1E-3</v>
@@ -4564,7 +4582,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -4582,7 +4600,7 @@
         <v>12</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K62" s="1">
         <v>1E-3</v>
@@ -4621,7 +4639,7 @@
         <v>2</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
@@ -4639,7 +4657,7 @@
         <v>12</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K63" s="1">
         <v>1E-3</v>
@@ -4674,16 +4692,16 @@
       <c r="B64" s="4">
         <v>10</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="1">
         <v>2</v>
       </c>
       <c r="D64" s="4">
         <v>20</v>
       </c>
-      <c r="E64" s="10">
-        <v>0</v>
-      </c>
-      <c r="F64" s="10">
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
         <v>0.3</v>
       </c>
       <c r="G64" s="4">
@@ -4692,19 +4710,19 @@
       <c r="H64" s="4">
         <v>100</v>
       </c>
-      <c r="I64" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J64" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K64" s="10">
+      <c r="I64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K64" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L64" s="10">
-        <v>0</v>
-      </c>
-      <c r="M64" s="10">
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
+      <c r="M64" s="1">
         <v>0</v>
       </c>
       <c r="N64" s="4">
@@ -4723,10 +4741,364 @@
         <v>0.93379999999999996</v>
       </c>
       <c r="S64" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T64" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="T64" s="2" t="s">
+    </row>
+    <row r="65" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>61</v>
+      </c>
+      <c r="B65" s="10">
+        <v>10</v>
+      </c>
+      <c r="C65" s="10">
+        <v>2</v>
+      </c>
+      <c r="D65" s="4">
+        <v>50</v>
+      </c>
+      <c r="E65" s="10">
+        <v>0</v>
+      </c>
+      <c r="F65" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G65" s="4">
+        <v>7461</v>
+      </c>
+      <c r="H65" s="10">
+        <v>100</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K65" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L65" s="10">
+        <v>0</v>
+      </c>
+      <c r="M65" s="10">
+        <v>0</v>
+      </c>
+      <c r="N65" s="10">
+        <v>16</v>
+      </c>
+      <c r="O65" s="2">
+        <v>98</v>
+      </c>
+      <c r="P65" s="2">
+        <v>49</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>29</v>
+      </c>
+      <c r="R65" s="8">
+        <v>0.82720000000000005</v>
+      </c>
+      <c r="T65" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>62</v>
+      </c>
+      <c r="B66" s="4">
+        <v>25</v>
+      </c>
+      <c r="C66" s="10">
+        <v>2</v>
+      </c>
+      <c r="D66" s="10">
+        <v>50</v>
+      </c>
+      <c r="E66" s="10">
+        <v>0</v>
+      </c>
+      <c r="F66" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G66" s="4">
+        <v>17666</v>
+      </c>
+      <c r="H66" s="10">
+        <v>100</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K66" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L66" s="10">
+        <v>0</v>
+      </c>
+      <c r="M66" s="10">
+        <v>0</v>
+      </c>
+      <c r="N66" s="10">
+        <v>16</v>
+      </c>
+      <c r="O66" s="2">
+        <v>94</v>
+      </c>
+      <c r="P66" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>70</v>
+      </c>
+      <c r="R66" s="8">
+        <v>0.5665</v>
+      </c>
+      <c r="T66" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>63</v>
+      </c>
+      <c r="B67" s="4">
+        <v>50</v>
+      </c>
+      <c r="C67" s="10">
+        <v>2</v>
+      </c>
+      <c r="D67" s="10">
+        <v>50</v>
+      </c>
+      <c r="E67" s="10">
+        <v>0</v>
+      </c>
+      <c r="F67" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G67" s="4">
+        <v>34000</v>
+      </c>
+      <c r="H67" s="10">
+        <v>100</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K67" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L67" s="10">
+        <v>0</v>
+      </c>
+      <c r="M67" s="10">
+        <v>0</v>
+      </c>
+      <c r="N67" s="10">
+        <v>16</v>
+      </c>
+      <c r="O67" s="2">
+        <v>84</v>
+      </c>
+      <c r="P67" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q67" s="2">
+        <v>66</v>
+      </c>
+      <c r="R67" s="8">
+        <v>0.35470000000000002</v>
+      </c>
+      <c r="T67" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>64</v>
+      </c>
+      <c r="B68" s="10">
+        <v>50</v>
+      </c>
+      <c r="C68" s="10">
+        <v>2</v>
+      </c>
+      <c r="D68" s="10">
+        <v>50</v>
+      </c>
+      <c r="E68" s="10">
+        <v>0</v>
+      </c>
+      <c r="F68" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G68" s="10">
+        <v>34000</v>
+      </c>
+      <c r="H68" s="10">
+        <v>100</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K68" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L68" s="10">
+        <v>0</v>
+      </c>
+      <c r="M68" s="10">
+        <v>0</v>
+      </c>
+      <c r="N68" s="4">
+        <v>64</v>
+      </c>
+      <c r="O68" s="2">
+        <v>86</v>
+      </c>
+      <c r="P68" s="2">
+        <v>22</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>23</v>
+      </c>
+      <c r="R68" s="8">
+        <v>0.38090000000000002</v>
+      </c>
+      <c r="T68" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>65</v>
+      </c>
+      <c r="B69" s="10">
+        <v>50</v>
+      </c>
+      <c r="C69" s="10">
+        <v>2</v>
+      </c>
+      <c r="D69" s="10">
+        <v>50</v>
+      </c>
+      <c r="E69" s="10">
+        <v>0</v>
+      </c>
+      <c r="F69" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G69" s="10">
+        <v>34000</v>
+      </c>
+      <c r="H69" s="4">
+        <v>500</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K69" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L69" s="10">
+        <v>0</v>
+      </c>
+      <c r="M69" s="10">
+        <v>0</v>
+      </c>
+      <c r="N69" s="10">
+        <v>64</v>
+      </c>
+      <c r="O69" s="2">
+        <v>98</v>
+      </c>
+      <c r="P69" s="2">
+        <v>22</v>
+      </c>
+      <c r="Q69" s="2">
+        <v>115</v>
+      </c>
+      <c r="R69" s="8">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="T69" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>66</v>
+      </c>
+      <c r="B70" s="10">
+        <v>50</v>
+      </c>
+      <c r="C70" s="10">
+        <v>2</v>
+      </c>
+      <c r="D70" s="4">
+        <v>100</v>
+      </c>
+      <c r="E70" s="10">
+        <v>0</v>
+      </c>
+      <c r="F70" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G70" s="10">
+        <v>34000</v>
+      </c>
+      <c r="H70" s="10">
+        <v>500</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K70" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L70" s="10">
+        <v>0</v>
+      </c>
+      <c r="M70" s="10">
+        <v>0</v>
+      </c>
+      <c r="N70" s="10">
+        <v>64</v>
+      </c>
+      <c r="O70" s="2">
+        <v>56</v>
+      </c>
+      <c r="P70" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>343</v>
+      </c>
+      <c r="R70" s="8">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="T70" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included median sampling technique
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66039F5A-9EDD-4C50-9445-066850CB4A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF036F00-A9FB-4AEE-808F-4D812D2A4517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="64">
   <si>
     <t>test number</t>
   </si>
@@ -248,9 +248,6 @@
     <t>[1, 50]</t>
   </si>
   <si>
-    <t>used TorchAudio instead of Librosa to load</t>
-  </si>
-  <si>
     <t>best_model_013.pth</t>
   </si>
   <si>
@@ -273,6 +270,22 @@
   </si>
   <si>
     <t>best_model_019.pth</t>
+  </si>
+  <si>
+    <t>best_model_020.pth</t>
+  </si>
+  <si>
+    <t>introduction of "median" sampling.
+"sound clips" is now the total sound clips
+AFTER sampling.</t>
+  </si>
+  <si>
+    <t>used TorchAudio instead of Librosa to load
+until next blue "other changes", all sound
+clips totals are BEFORE sampling</t>
+  </si>
+  <si>
+    <t>best_model_021.pth</t>
   </si>
 </sst>
 </file>
@@ -626,8 +639,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T70" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A2:T70" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:T72" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:T72" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S45">
     <sortCondition ref="A2:A45"/>
   </sortState>
@@ -954,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:T70"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G51" workbookViewId="0">
-      <selection activeCell="T71" sqref="T71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>6</v>
@@ -4685,7 +4698,7 @@
       </c>
       <c r="T63" s="2"/>
     </row>
-    <row r="64" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -4740,54 +4753,54 @@
       <c r="R64" s="8">
         <v>0.93379999999999996</v>
       </c>
-      <c r="S64" s="4" t="s">
+      <c r="S64" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T64" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="T64" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>61</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="1">
         <v>10</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="1">
         <v>2</v>
       </c>
       <c r="D65" s="4">
         <v>50</v>
       </c>
-      <c r="E65" s="10">
-        <v>0</v>
-      </c>
-      <c r="F65" s="10">
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
         <v>0.3</v>
       </c>
       <c r="G65" s="4">
         <v>7461</v>
       </c>
-      <c r="H65" s="10">
+      <c r="H65" s="1">
         <v>100</v>
       </c>
-      <c r="I65" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J65" s="10" t="s">
+      <c r="I65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K65" s="10">
+      <c r="K65" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L65" s="10">
-        <v>0</v>
-      </c>
-      <c r="M65" s="10">
-        <v>0</v>
-      </c>
-      <c r="N65" s="10">
+      <c r="L65" s="1">
+        <v>0</v>
+      </c>
+      <c r="M65" s="1">
+        <v>0</v>
+      </c>
+      <c r="N65" s="1">
         <v>16</v>
       </c>
       <c r="O65" s="2">
@@ -4803,7 +4816,7 @@
         <v>0.82720000000000005</v>
       </c>
       <c r="T65" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4813,40 +4826,40 @@
       <c r="B66" s="4">
         <v>25</v>
       </c>
-      <c r="C66" s="10">
-        <v>2</v>
-      </c>
-      <c r="D66" s="10">
+      <c r="C66" s="1">
+        <v>2</v>
+      </c>
+      <c r="D66" s="1">
         <v>50</v>
       </c>
-      <c r="E66" s="10">
-        <v>0</v>
-      </c>
-      <c r="F66" s="10">
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
         <v>0.3</v>
       </c>
       <c r="G66" s="4">
         <v>17666</v>
       </c>
-      <c r="H66" s="10">
+      <c r="H66" s="1">
         <v>100</v>
       </c>
-      <c r="I66" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J66" s="10" t="s">
+      <c r="I66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K66" s="10">
+      <c r="K66" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L66" s="10">
-        <v>0</v>
-      </c>
-      <c r="M66" s="10">
-        <v>0</v>
-      </c>
-      <c r="N66" s="10">
+      <c r="L66" s="1">
+        <v>0</v>
+      </c>
+      <c r="M66" s="1">
+        <v>0</v>
+      </c>
+      <c r="N66" s="1">
         <v>16</v>
       </c>
       <c r="O66" s="2">
@@ -4862,7 +4875,7 @@
         <v>0.5665</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -4872,40 +4885,40 @@
       <c r="B67" s="4">
         <v>50</v>
       </c>
-      <c r="C67" s="10">
-        <v>2</v>
-      </c>
-      <c r="D67" s="10">
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
         <v>50</v>
       </c>
-      <c r="E67" s="10">
-        <v>0</v>
-      </c>
-      <c r="F67" s="10">
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
         <v>0.3</v>
       </c>
       <c r="G67" s="4">
         <v>34000</v>
       </c>
-      <c r="H67" s="10">
+      <c r="H67" s="1">
         <v>100</v>
       </c>
-      <c r="I67" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J67" s="10" t="s">
+      <c r="I67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J67" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K67" s="10">
+      <c r="K67" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L67" s="10">
-        <v>0</v>
-      </c>
-      <c r="M67" s="10">
-        <v>0</v>
-      </c>
-      <c r="N67" s="10">
+      <c r="L67" s="1">
+        <v>0</v>
+      </c>
+      <c r="M67" s="1">
+        <v>0</v>
+      </c>
+      <c r="N67" s="1">
         <v>16</v>
       </c>
       <c r="O67" s="2">
@@ -4921,47 +4934,47 @@
         <v>0.35470000000000002</v>
       </c>
       <c r="T67" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>64</v>
       </c>
-      <c r="B68" s="10">
+      <c r="B68" s="1">
         <v>50</v>
       </c>
-      <c r="C68" s="10">
-        <v>2</v>
-      </c>
-      <c r="D68" s="10">
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
         <v>50</v>
       </c>
-      <c r="E68" s="10">
-        <v>0</v>
-      </c>
-      <c r="F68" s="10">
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
         <v>0.3</v>
       </c>
-      <c r="G68" s="10">
+      <c r="G68" s="1">
         <v>34000</v>
       </c>
-      <c r="H68" s="10">
+      <c r="H68" s="1">
         <v>100</v>
       </c>
-      <c r="I68" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J68" s="10" t="s">
+      <c r="I68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K68" s="10">
+      <c r="K68" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L68" s="10">
-        <v>0</v>
-      </c>
-      <c r="M68" s="10">
+      <c r="L68" s="1">
+        <v>0</v>
+      </c>
+      <c r="M68" s="1">
         <v>0</v>
       </c>
       <c r="N68" s="4">
@@ -4980,50 +4993,50 @@
         <v>0.38090000000000002</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>65</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="1">
         <v>50</v>
       </c>
-      <c r="C69" s="10">
-        <v>2</v>
-      </c>
-      <c r="D69" s="10">
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
         <v>50</v>
       </c>
-      <c r="E69" s="10">
-        <v>0</v>
-      </c>
-      <c r="F69" s="10">
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
         <v>0.3</v>
       </c>
-      <c r="G69" s="10">
+      <c r="G69" s="1">
         <v>34000</v>
       </c>
       <c r="H69" s="4">
         <v>500</v>
       </c>
-      <c r="I69" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J69" s="10" t="s">
+      <c r="I69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J69" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K69" s="10">
+      <c r="K69" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L69" s="10">
-        <v>0</v>
-      </c>
-      <c r="M69" s="10">
-        <v>0</v>
-      </c>
-      <c r="N69" s="10">
+      <c r="L69" s="1">
+        <v>0</v>
+      </c>
+      <c r="M69" s="1">
+        <v>0</v>
+      </c>
+      <c r="N69" s="1">
         <v>64</v>
       </c>
       <c r="O69" s="2">
@@ -5039,50 +5052,50 @@
         <v>0.35289999999999999</v>
       </c>
       <c r="T69" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>66</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="1">
         <v>50</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="1">
         <v>2</v>
       </c>
       <c r="D70" s="4">
         <v>100</v>
       </c>
-      <c r="E70" s="10">
-        <v>0</v>
-      </c>
-      <c r="F70" s="10">
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
         <v>0.3</v>
       </c>
-      <c r="G70" s="10">
+      <c r="G70" s="1">
         <v>34000</v>
       </c>
-      <c r="H70" s="10">
+      <c r="H70" s="1">
         <v>500</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J70" s="10" t="s">
+      <c r="I70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K70" s="10">
+      <c r="K70" s="1">
         <v>1E-3</v>
       </c>
-      <c r="L70" s="10">
-        <v>0</v>
-      </c>
-      <c r="M70" s="10">
-        <v>0</v>
-      </c>
-      <c r="N70" s="10">
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
         <v>64</v>
       </c>
       <c r="O70" s="2">
@@ -5098,7 +5111,128 @@
         <v>0.43640000000000001</v>
       </c>
       <c r="T70" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>67</v>
+      </c>
+      <c r="B71" s="1">
+        <v>50</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2</v>
+      </c>
+      <c r="D71" s="10">
+        <v>100</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G71" s="4">
+        <v>66124</v>
+      </c>
+      <c r="H71" s="1">
+        <v>500</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K71" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L71" s="1">
+        <v>0</v>
+      </c>
+      <c r="M71" s="1">
+        <v>0</v>
+      </c>
+      <c r="N71" s="1">
+        <v>64</v>
+      </c>
+      <c r="O71" s="2">
+        <v>54</v>
+      </c>
+      <c r="P71" s="2">
+        <v>22</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>352</v>
+      </c>
+      <c r="R71" s="8">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="T71" s="2" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>68</v>
+      </c>
+      <c r="B72" s="10">
+        <v>50</v>
+      </c>
+      <c r="C72" s="10">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>100</v>
+      </c>
+      <c r="E72" s="10">
+        <v>0</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G72" s="4">
+        <v>58000</v>
+      </c>
+      <c r="H72" s="10">
+        <v>500</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K72" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="L72" s="10">
+        <v>0</v>
+      </c>
+      <c r="M72" s="10">
+        <v>0</v>
+      </c>
+      <c r="N72" s="10">
+        <v>64</v>
+      </c>
+      <c r="O72" s="2">
+        <v>37</v>
+      </c>
+      <c r="P72" s="2">
+        <v>26</v>
+      </c>
+      <c r="Q72" s="2">
+        <v>1154</v>
+      </c>
+      <c r="R72" s="8">
+        <v>0.53259999999999996</v>
+      </c>
+      <c r="S72" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T72" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cnn test results for sciama
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A8434D-257C-4AF1-BC68-4745B9887DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1015B6-F1A2-471C-9B2A-70EF604A1125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="75">
   <si>
     <t>test number</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>best_model_022.pth</t>
+  </si>
+  <si>
+    <t>best_model_023.pth</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -409,22 +415,85 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="36">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -450,6 +519,25 @@
     <dxf>
       <font>
         <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -465,25 +553,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -626,6 +695,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -692,34 +764,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:V73" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A2:V73" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:V75" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A2:V75" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:U45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="8"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="28"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="16"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1022,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="F54" workbookViewId="0">
+      <selection activeCell="S76" sqref="S76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,26 +1127,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -3257,7 +3329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -3315,7 +3387,7 @@
       <c r="S35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T35" s="10" t="s">
+      <c r="T35" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U35" s="5" t="s">
@@ -3721,7 +3793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -3779,7 +3851,7 @@
       <c r="S42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T42" s="10" t="s">
+      <c r="T42" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U42" s="6" t="s">
@@ -3789,7 +3861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -3857,7 +3929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -3991,7 +4063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -4655,7 +4727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -4723,7 +4795,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -4915,7 +4987,7 @@
       <c r="S59" s="8">
         <v>0.87439999999999996</v>
       </c>
-      <c r="T59" s="10" t="s">
+      <c r="T59" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U59" s="4" t="s">
@@ -5179,7 +5251,7 @@
       <c r="U63" s="1"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -5237,7 +5309,7 @@
       <c r="S64" s="8">
         <v>0.93379999999999996</v>
       </c>
-      <c r="T64" s="11" t="s">
+      <c r="T64" s="10" t="s">
         <v>66</v>
       </c>
       <c r="U64" s="6" t="s">
@@ -5709,7 +5781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -5728,7 +5800,7 @@
       <c r="F72" s="1">
         <v>0.2</v>
       </c>
-      <c r="G72" s="1" t="s">
+      <c r="G72" s="4" t="s">
         <v>72</v>
       </c>
       <c r="H72" s="4">
@@ -5835,11 +5907,143 @@
       <c r="S73" s="8">
         <v>0.46870000000000001</v>
       </c>
-      <c r="T73" s="10" t="s">
+      <c r="T73" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U73" s="1"/>
       <c r="V73" s="2"/>
+    </row>
+    <row r="74" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>70</v>
+      </c>
+      <c r="B74" s="1">
+        <v>50</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1">
+        <v>100</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H74" s="4">
+        <v>63750</v>
+      </c>
+      <c r="I74" s="1">
+        <v>500</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L74" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M74" s="1">
+        <v>0</v>
+      </c>
+      <c r="N74" s="1">
+        <v>0</v>
+      </c>
+      <c r="O74" s="1">
+        <v>64</v>
+      </c>
+      <c r="P74" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>23</v>
+      </c>
+      <c r="R74" s="2">
+        <v>1175</v>
+      </c>
+      <c r="S74" s="8">
+        <v>0.50280000000000002</v>
+      </c>
+      <c r="T74" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U74" s="1"/>
+      <c r="V74" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>71</v>
+      </c>
+      <c r="B75" s="12">
+        <v>50</v>
+      </c>
+      <c r="C75" s="12">
+        <v>2</v>
+      </c>
+      <c r="D75" s="1">
+        <v>100</v>
+      </c>
+      <c r="E75" s="12">
+        <v>0</v>
+      </c>
+      <c r="F75" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H75" s="4">
+        <v>65650</v>
+      </c>
+      <c r="I75" s="12">
+        <v>500</v>
+      </c>
+      <c r="J75" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L75" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="M75" s="12">
+        <v>0</v>
+      </c>
+      <c r="N75" s="12">
+        <v>0</v>
+      </c>
+      <c r="O75" s="12">
+        <v>64</v>
+      </c>
+      <c r="P75" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>24</v>
+      </c>
+      <c r="R75" s="2">
+        <v>1213</v>
+      </c>
+      <c r="S75" s="8">
+        <v>0.50939999999999996</v>
+      </c>
+      <c r="T75" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U75" s="1"/>
+      <c r="V75" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5847,17 +6051,17 @@
     <mergeCell ref="B1:N1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="O1 O74:O1048576 P2:P73">
+  <conditionalFormatting sqref="P2:P75">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.01</formula>
+      <formula>80</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
-      <formula>0.01</formula>
-      <formula>80</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
experimentation with sequential aggregation strategy
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1015B6-F1A2-471C-9B2A-70EF604A1125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D01498-5CD3-4502-BAF2-3468DF0A0053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -325,7 +325,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +357,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,91 +416,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="27">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -520,48 +506,6 @@
       <font>
         <b/>
         <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -764,34 +708,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:V75" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:V75" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A2:V75" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:U45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="31"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="28"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="16"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1096,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F54" workbookViewId="0">
-      <selection activeCell="S76" sqref="S76"/>
+    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,27 +1071,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="P1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="7"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1275,7 +1219,7 @@
       <c r="S3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U3" s="1"/>
@@ -1341,7 +1285,7 @@
       <c r="S4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U4" s="1"/>
@@ -1407,7 +1351,7 @@
       <c r="S5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U5" s="1"/>
@@ -1473,7 +1417,7 @@
       <c r="S6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U6" s="1"/>
@@ -1539,7 +1483,7 @@
       <c r="S7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U7" s="1"/>
@@ -1605,7 +1549,7 @@
       <c r="S8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U8" s="1"/>
@@ -1671,7 +1615,7 @@
       <c r="S9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U9" s="1"/>
@@ -1737,7 +1681,7 @@
       <c r="S10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U10" s="1"/>
@@ -1803,7 +1747,7 @@
       <c r="S11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U11" s="1"/>
@@ -1869,7 +1813,7 @@
       <c r="S12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U12" s="1"/>
@@ -1935,7 +1879,7 @@
       <c r="S13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U13" s="1"/>
@@ -2001,7 +1945,7 @@
       <c r="S14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U14" s="1"/>
@@ -2067,7 +2011,7 @@
       <c r="S15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="T15" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U15" s="1"/>
@@ -2133,7 +2077,7 @@
       <c r="S16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="T16" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U16" s="1"/>
@@ -2199,7 +2143,7 @@
       <c r="S17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U17" s="1"/>
@@ -2265,7 +2209,7 @@
       <c r="S18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U18" s="1"/>
@@ -2331,7 +2275,7 @@
       <c r="S19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="T19" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U19" s="1"/>
@@ -2397,7 +2341,7 @@
       <c r="S20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U20" s="1"/>
@@ -2463,7 +2407,7 @@
       <c r="S21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U21" s="1"/>
@@ -2529,7 +2473,7 @@
       <c r="S22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="T22" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U22" s="1"/>
@@ -2595,7 +2539,7 @@
       <c r="S23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="T23" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U23" s="1"/>
@@ -2661,7 +2605,7 @@
       <c r="S24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T24" s="2" t="s">
+      <c r="T24" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U24" s="1"/>
@@ -2727,7 +2671,7 @@
       <c r="S25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T25" s="2" t="s">
+      <c r="T25" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U25" s="1"/>
@@ -2793,7 +2737,7 @@
       <c r="S26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="T26" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U26" s="1"/>
@@ -2859,7 +2803,7 @@
       <c r="S27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="T27" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U27" s="1"/>
@@ -2925,7 +2869,7 @@
       <c r="S28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="T28" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U28" s="1"/>
@@ -2991,7 +2935,7 @@
       <c r="S29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="T29" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U29" s="1"/>
@@ -3057,7 +3001,7 @@
       <c r="S30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="T30" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U30" s="1"/>
@@ -3123,7 +3067,7 @@
       <c r="S31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="T31" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U31" s="1"/>
@@ -3189,7 +3133,7 @@
       <c r="S32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="T32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U32" s="1"/>
@@ -3255,7 +3199,7 @@
       <c r="S33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T33" s="2" t="s">
+      <c r="T33" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U33" s="1"/>
@@ -3321,7 +3265,7 @@
       <c r="S34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T34" s="2" t="s">
+      <c r="T34" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U34" s="1"/>
@@ -3387,7 +3331,7 @@
       <c r="S35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T35" s="9" t="s">
+      <c r="T35" s="10" t="s">
         <v>67</v>
       </c>
       <c r="U35" s="5" t="s">
@@ -3455,7 +3399,7 @@
       <c r="S36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T36" s="2" t="s">
+      <c r="T36" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U36" s="1"/>
@@ -3521,7 +3465,7 @@
       <c r="S37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T37" s="2" t="s">
+      <c r="T37" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U37" s="1"/>
@@ -3587,7 +3531,7 @@
       <c r="S38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T38" s="2" t="s">
+      <c r="T38" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U38" s="1"/>
@@ -3653,7 +3597,7 @@
       <c r="S39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T39" s="2" t="s">
+      <c r="T39" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U39" s="1"/>
@@ -3719,7 +3663,7 @@
       <c r="S40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T40" s="2" t="s">
+      <c r="T40" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U40" s="1"/>
@@ -3785,7 +3729,7 @@
       <c r="S41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T41" s="2" t="s">
+      <c r="T41" s="9" t="s">
         <v>67</v>
       </c>
       <c r="U41" s="1"/>
@@ -3851,7 +3795,7 @@
       <c r="S42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T42" s="9" t="s">
+      <c r="T42" s="10" t="s">
         <v>66</v>
       </c>
       <c r="U42" s="6" t="s">
@@ -3919,7 +3863,7 @@
       <c r="S43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T43" s="2" t="s">
+      <c r="T43" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U43" s="6" t="s">
@@ -3987,7 +3931,7 @@
       <c r="S44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T44" s="2" t="s">
+      <c r="T44" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U44" s="6" t="s">
@@ -4055,7 +3999,7 @@
       <c r="S45" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T45" s="2" t="s">
+      <c r="T45" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U45" s="1"/>
@@ -4121,7 +4065,7 @@
       <c r="S46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T46" s="2" t="s">
+      <c r="T46" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U46" s="6" t="s">
@@ -4186,10 +4130,10 @@
       <c r="R47" s="2">
         <v>523</v>
       </c>
-      <c r="S47" s="8">
+      <c r="S47" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="T47" s="2" t="s">
+      <c r="T47" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U47" s="4" t="s">
@@ -4257,7 +4201,7 @@
       <c r="S48" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T48" s="2" t="s">
+      <c r="T48" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U48" s="1"/>
@@ -4320,10 +4264,10 @@
       <c r="R49" s="2">
         <v>393</v>
       </c>
-      <c r="S49" s="8">
+      <c r="S49" s="7">
         <v>0.81869999999999998</v>
       </c>
-      <c r="T49" s="2" t="s">
+      <c r="T49" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U49" s="1"/>
@@ -4386,10 +4330,10 @@
       <c r="R50" s="2">
         <v>389</v>
       </c>
-      <c r="S50" s="8">
+      <c r="S50" s="7">
         <v>0.68720000000000003</v>
       </c>
-      <c r="T50" s="2" t="s">
+      <c r="T50" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U50" s="1"/>
@@ -4452,10 +4396,10 @@
       <c r="R51" s="2">
         <v>393</v>
       </c>
-      <c r="S51" s="8">
+      <c r="S51" s="7">
         <v>0.76029999999999998</v>
       </c>
-      <c r="T51" s="2" t="s">
+      <c r="T51" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U51" s="1"/>
@@ -4518,10 +4462,10 @@
       <c r="R52" s="2">
         <v>400</v>
       </c>
-      <c r="S52" s="8">
+      <c r="S52" s="7">
         <v>0.6452</v>
       </c>
-      <c r="T52" s="2" t="s">
+      <c r="T52" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U52" s="1"/>
@@ -4584,10 +4528,10 @@
       <c r="R53" s="2">
         <v>721</v>
       </c>
-      <c r="S53" s="8">
+      <c r="S53" s="7">
         <v>0.72209999999999996</v>
       </c>
-      <c r="T53" s="2" t="s">
+      <c r="T53" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U53" s="1"/>
@@ -4650,10 +4594,10 @@
       <c r="R54" s="2">
         <v>546</v>
       </c>
-      <c r="S54" s="8">
+      <c r="S54" s="7">
         <v>0.7097</v>
       </c>
-      <c r="T54" s="2" t="s">
+      <c r="T54" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U54" s="1"/>
@@ -4716,10 +4660,10 @@
       <c r="R55" s="2">
         <v>541</v>
       </c>
-      <c r="S55" s="8">
+      <c r="S55" s="7">
         <v>0.73860000000000003</v>
       </c>
-      <c r="T55" s="2" t="s">
+      <c r="T55" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U55" s="1"/>
@@ -4782,10 +4726,10 @@
       <c r="R56" s="2">
         <v>1050</v>
       </c>
-      <c r="S56" s="8">
+      <c r="S56" s="7">
         <v>0.76690000000000003</v>
       </c>
-      <c r="T56" s="2" t="s">
+      <c r="T56" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U56" s="6" t="s">
@@ -4850,10 +4794,10 @@
       <c r="R57" s="2">
         <v>592</v>
       </c>
-      <c r="S57" s="8">
+      <c r="S57" s="7">
         <v>0.71640000000000004</v>
       </c>
-      <c r="T57" s="2" t="s">
+      <c r="T57" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U57" s="6" t="s">
@@ -4918,10 +4862,10 @@
       <c r="R58" s="2">
         <v>604</v>
       </c>
-      <c r="S58" s="8">
+      <c r="S58" s="7">
         <v>0.78759999999999997</v>
       </c>
-      <c r="T58" s="2" t="s">
+      <c r="T58" s="9" t="s">
         <v>66</v>
       </c>
       <c r="U58" s="1"/>
@@ -4984,10 +4928,10 @@
       <c r="R59" s="2">
         <v>45</v>
       </c>
-      <c r="S59" s="8">
+      <c r="S59" s="7">
         <v>0.87439999999999996</v>
       </c>
-      <c r="T59" s="9" t="s">
+      <c r="T59" s="10" t="s">
         <v>65</v>
       </c>
       <c r="U59" s="4" t="s">
@@ -5050,10 +4994,10 @@
       <c r="R60" s="2">
         <v>61</v>
       </c>
-      <c r="S60" s="8">
+      <c r="S60" s="7">
         <v>0.96299999999999997</v>
       </c>
-      <c r="T60" s="2" t="s">
+      <c r="T60" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U60" s="1"/>
@@ -5114,10 +5058,10 @@
       <c r="R61" s="2">
         <v>13</v>
       </c>
-      <c r="S61" s="8">
+      <c r="S61" s="7">
         <v>0.96199999999999997</v>
       </c>
-      <c r="T61" s="2" t="s">
+      <c r="T61" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U61" s="1"/>
@@ -5178,10 +5122,10 @@
       <c r="R62" s="2">
         <v>48</v>
       </c>
-      <c r="S62" s="8">
+      <c r="S62" s="7">
         <v>0.97460000000000002</v>
       </c>
-      <c r="T62" s="2" t="s">
+      <c r="T62" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U62" s="1"/>
@@ -5242,10 +5186,10 @@
       <c r="R63" s="2">
         <v>88</v>
       </c>
-      <c r="S63" s="8">
+      <c r="S63" s="7">
         <v>0.89070000000000005</v>
       </c>
-      <c r="T63" s="2" t="s">
+      <c r="T63" s="9" t="s">
         <v>65</v>
       </c>
       <c r="U63" s="1"/>
@@ -5306,10 +5250,10 @@
       <c r="R64" s="2">
         <v>104</v>
       </c>
-      <c r="S64" s="8">
+      <c r="S64" s="7">
         <v>0.93379999999999996</v>
       </c>
-      <c r="T64" s="10" t="s">
+      <c r="T64" s="11" t="s">
         <v>66</v>
       </c>
       <c r="U64" s="6" t="s">
@@ -5374,10 +5318,10 @@
       <c r="R65" s="2">
         <v>29</v>
       </c>
-      <c r="S65" s="8">
+      <c r="S65" s="7">
         <v>0.82720000000000005</v>
       </c>
-      <c r="T65" s="8" t="s">
+      <c r="T65" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U65" s="1"/>
@@ -5440,10 +5384,10 @@
       <c r="R66" s="2">
         <v>70</v>
       </c>
-      <c r="S66" s="8">
+      <c r="S66" s="7">
         <v>0.5665</v>
       </c>
-      <c r="T66" s="8" t="s">
+      <c r="T66" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U66" s="1"/>
@@ -5506,10 +5450,10 @@
       <c r="R67" s="2">
         <v>66</v>
       </c>
-      <c r="S67" s="8">
+      <c r="S67" s="7">
         <v>0.35470000000000002</v>
       </c>
-      <c r="T67" s="8" t="s">
+      <c r="T67" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U67" s="1"/>
@@ -5572,10 +5516,10 @@
       <c r="R68" s="2">
         <v>23</v>
       </c>
-      <c r="S68" s="8">
+      <c r="S68" s="7">
         <v>0.38090000000000002</v>
       </c>
-      <c r="T68" s="8" t="s">
+      <c r="T68" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U68" s="1"/>
@@ -5638,10 +5582,10 @@
       <c r="R69" s="2">
         <v>115</v>
       </c>
-      <c r="S69" s="8">
+      <c r="S69" s="7">
         <v>0.35289999999999999</v>
       </c>
-      <c r="T69" s="8" t="s">
+      <c r="T69" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U69" s="1"/>
@@ -5704,10 +5648,10 @@
       <c r="R70" s="2">
         <v>343</v>
       </c>
-      <c r="S70" s="8">
+      <c r="S70" s="7">
         <v>0.43640000000000001</v>
       </c>
-      <c r="T70" s="8" t="s">
+      <c r="T70" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U70" s="1"/>
@@ -5770,10 +5714,10 @@
       <c r="R71" s="2">
         <v>352</v>
       </c>
-      <c r="S71" s="8">
+      <c r="S71" s="7">
         <v>0.43209999999999998</v>
       </c>
-      <c r="T71" s="8" t="s">
+      <c r="T71" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U71" s="1"/>
@@ -5836,10 +5780,10 @@
       <c r="R72" s="2">
         <v>1154</v>
       </c>
-      <c r="S72" s="8">
+      <c r="S72" s="7">
         <v>0.53259999999999996</v>
       </c>
-      <c r="T72" s="8" t="s">
+      <c r="T72" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U72" s="6" t="s">
@@ -5904,10 +5848,10 @@
       <c r="R73" s="2">
         <v>499</v>
       </c>
-      <c r="S73" s="8">
+      <c r="S73" s="7">
         <v>0.46870000000000001</v>
       </c>
-      <c r="T73" s="9" t="s">
+      <c r="T73" s="10" t="s">
         <v>65</v>
       </c>
       <c r="U73" s="1"/>
@@ -5968,10 +5912,10 @@
       <c r="R74" s="2">
         <v>1175</v>
       </c>
-      <c r="S74" s="8">
+      <c r="S74" s="7">
         <v>0.50280000000000002</v>
       </c>
-      <c r="T74" s="8" t="s">
+      <c r="T74" s="12" t="s">
         <v>65</v>
       </c>
       <c r="U74" s="1"/>
@@ -5983,19 +5927,19 @@
       <c r="A75" s="1">
         <v>71</v>
       </c>
-      <c r="B75" s="12">
+      <c r="B75" s="1">
         <v>50</v>
       </c>
-      <c r="C75" s="12">
+      <c r="C75" s="1">
         <v>2</v>
       </c>
       <c r="D75" s="1">
         <v>100</v>
       </c>
-      <c r="E75" s="12">
-        <v>0</v>
-      </c>
-      <c r="F75" s="12">
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1">
         <v>0.2</v>
       </c>
       <c r="G75" s="1" t="s">
@@ -6004,25 +5948,25 @@
       <c r="H75" s="4">
         <v>65650</v>
       </c>
-      <c r="I75" s="12">
+      <c r="I75" s="1">
         <v>500</v>
       </c>
-      <c r="J75" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="K75" s="12" t="s">
+      <c r="J75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L75" s="12">
+      <c r="L75" s="1">
         <v>1E-3</v>
       </c>
-      <c r="M75" s="12">
-        <v>0</v>
-      </c>
-      <c r="N75" s="12">
-        <v>0</v>
-      </c>
-      <c r="O75" s="12">
+      <c r="M75" s="1">
+        <v>0</v>
+      </c>
+      <c r="N75" s="1">
+        <v>0</v>
+      </c>
+      <c r="O75" s="1">
         <v>64</v>
       </c>
       <c r="P75" s="2">
@@ -6034,10 +5978,10 @@
       <c r="R75" s="2">
         <v>1213</v>
       </c>
-      <c r="S75" s="8">
+      <c r="S75" s="7">
         <v>0.50939999999999996</v>
       </c>
-      <c r="T75" s="8" t="s">
+      <c r="T75" s="12" t="s">
         <v>65</v>
       </c>
       <c r="U75" s="1"/>
@@ -6047,21 +5991,21 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="B1:N1"/>
+    <mergeCell ref="P1:S1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="P2:P75">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>100</formula>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+      <formula>90</formula>
+      <formula>99</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
-      <formula>90</formula>
-      <formula>99</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
introduction of extra techniques. check test results
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8593584-D971-4748-B235-E0359DD4AE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9807ABA-9F92-4AFB-ABB0-12C38999EBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="91">
   <si>
     <t>test number</t>
   </si>
@@ -353,11 +353,34 @@
   <si>
     <t>4.0-5.0</t>
   </si>
+  <si>
+    <t>5.0-5.0</t>
+  </si>
+  <si>
+    <t>best_model_038.pth</t>
+  </si>
+  <si>
+    <t>introduction of experimental epoch training
+stops training after 5 consecutive epochs of no
+updates to testing accuracy.</t>
+  </si>
+  <si>
+    <t>500 (48)</t>
+  </si>
+  <si>
+    <t>best_model_039.pth</t>
+  </si>
+  <si>
+    <t>best_model_040.pth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -470,50 +493,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <fill>
         <patternFill>
@@ -790,6 +777,24 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
@@ -825,36 +830,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X80" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="A2:X80" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X82" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A2:X82" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:X76">
     <sortCondition ref="B2:B80"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="0"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="31"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="30"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="15"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="31"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="30"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1157,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:X80"/>
+  <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="K70" workbookViewId="0">
+      <selection activeCell="U82" sqref="U82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6566,16 +6571,16 @@
       <c r="D76" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E76" s="13">
+      <c r="E76" s="1">
         <v>2</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
       </c>
-      <c r="G76" s="13">
-        <v>0</v>
-      </c>
-      <c r="H76" s="13">
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
         <v>0.2</v>
       </c>
       <c r="I76" s="1" t="s">
@@ -6584,25 +6589,25 @@
       <c r="J76" s="4">
         <v>4820</v>
       </c>
-      <c r="K76" s="13">
+      <c r="K76" s="1">
         <v>500</v>
       </c>
-      <c r="L76" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M76" s="13" t="s">
+      <c r="L76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M76" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N76" s="13">
+      <c r="N76" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O76" s="13">
-        <v>0</v>
-      </c>
-      <c r="P76" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q76" s="13">
+      <c r="O76" s="1">
+        <v>0</v>
+      </c>
+      <c r="P76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="1">
         <v>64</v>
       </c>
       <c r="R76" s="2">
@@ -6632,22 +6637,22 @@
       <c r="B77" s="4">
         <v>25</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E77" s="13">
+      <c r="E77" s="1">
         <v>2</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
       </c>
-      <c r="G77" s="13">
-        <v>0</v>
-      </c>
-      <c r="H77" s="13">
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
         <v>0.2</v>
       </c>
       <c r="I77" s="1" t="s">
@@ -6656,25 +6661,25 @@
       <c r="J77" s="4">
         <v>12300</v>
       </c>
-      <c r="K77" s="13">
+      <c r="K77" s="1">
         <v>500</v>
       </c>
-      <c r="L77" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M77" s="13" t="s">
+      <c r="L77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M77" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N77" s="13">
+      <c r="N77" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O77" s="13">
-        <v>0</v>
-      </c>
-      <c r="P77" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q77" s="13">
+      <c r="O77" s="1">
+        <v>0</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1">
         <v>64</v>
       </c>
       <c r="R77" s="2">
@@ -6704,49 +6709,49 @@
       <c r="B78" s="4">
         <v>50</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E78" s="13">
+      <c r="E78" s="1">
         <v>2</v>
       </c>
       <c r="F78" s="4">
         <v>100</v>
       </c>
-      <c r="G78" s="13">
-        <v>0</v>
-      </c>
-      <c r="H78" s="13">
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
         <v>0.2</v>
       </c>
-      <c r="I78" s="13" t="s">
+      <c r="I78" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J78" s="4">
         <v>26200</v>
       </c>
-      <c r="K78" s="13">
+      <c r="K78" s="1">
         <v>500</v>
       </c>
-      <c r="L78" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M78" s="13" t="s">
+      <c r="L78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M78" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N78" s="13">
+      <c r="N78" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O78" s="13">
-        <v>0</v>
-      </c>
-      <c r="P78" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q78" s="13">
+      <c r="O78" s="1">
+        <v>0</v>
+      </c>
+      <c r="P78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="1">
         <v>64</v>
       </c>
       <c r="R78" s="2">
@@ -6776,49 +6781,49 @@
       <c r="B79" s="4">
         <v>100</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E79" s="13">
+      <c r="E79" s="1">
         <v>2</v>
       </c>
       <c r="F79" s="1">
         <v>100</v>
       </c>
-      <c r="G79" s="13">
-        <v>0</v>
-      </c>
-      <c r="H79" s="13">
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
         <v>0.2</v>
       </c>
-      <c r="I79" s="13" t="s">
+      <c r="I79" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J79" s="4">
         <v>45100</v>
       </c>
-      <c r="K79" s="13">
+      <c r="K79" s="1">
         <v>500</v>
       </c>
-      <c r="L79" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M79" s="13" t="s">
+      <c r="L79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M79" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N79" s="13">
+      <c r="N79" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O79" s="13">
-        <v>0</v>
-      </c>
-      <c r="P79" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q79" s="13">
+      <c r="O79" s="1">
+        <v>0</v>
+      </c>
+      <c r="P79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="1">
         <v>64</v>
       </c>
       <c r="R79" s="2">
@@ -6845,52 +6850,52 @@
       <c r="A80" s="1">
         <v>76</v>
       </c>
-      <c r="B80" s="13">
+      <c r="B80" s="1">
         <v>100</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="13" t="s">
+      <c r="D80" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E80" s="13">
+      <c r="E80" s="1">
         <v>2</v>
       </c>
       <c r="F80" s="4">
         <v>50</v>
       </c>
-      <c r="G80" s="13">
-        <v>0</v>
-      </c>
-      <c r="H80" s="13">
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
         <v>0.2</v>
       </c>
-      <c r="I80" s="13" t="s">
+      <c r="I80" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J80" s="4">
         <v>41900</v>
       </c>
-      <c r="K80" s="13">
+      <c r="K80" s="1">
         <v>500</v>
       </c>
-      <c r="L80" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M80" s="13" t="s">
+      <c r="L80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M80" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N80" s="13">
+      <c r="N80" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O80" s="13">
-        <v>0</v>
-      </c>
-      <c r="P80" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q80" s="13">
+      <c r="O80" s="1">
+        <v>0</v>
+      </c>
+      <c r="P80" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="1">
         <v>64</v>
       </c>
       <c r="R80" s="2">
@@ -6905,9 +6910,159 @@
       <c r="U80" s="7">
         <v>0.6</v>
       </c>
-      <c r="V80" s="11"/>
+      <c r="V80" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="W80" s="1"/>
-      <c r="X80" s="2"/>
+      <c r="X80" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>77</v>
+      </c>
+      <c r="B81" s="13">
+        <v>200</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E81" s="13">
+        <v>2</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="13">
+        <v>0</v>
+      </c>
+      <c r="H81" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J81" s="4">
+        <v>108400</v>
+      </c>
+      <c r="K81" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="L81" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M81" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N81" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="O81" s="13">
+        <v>0</v>
+      </c>
+      <c r="P81" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>64</v>
+      </c>
+      <c r="R81" s="2">
+        <v>26</v>
+      </c>
+      <c r="S81" s="2">
+        <v>22</v>
+      </c>
+      <c r="T81" s="2">
+        <v>990</v>
+      </c>
+      <c r="U81" s="7">
+        <v>0.40489999999999998</v>
+      </c>
+      <c r="V81" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W81" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X81" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>78</v>
+      </c>
+      <c r="B82" s="4">
+        <v>100</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E82" s="13">
+        <v>2</v>
+      </c>
+      <c r="F82" s="4">
+        <v>100</v>
+      </c>
+      <c r="G82" s="13">
+        <v>0</v>
+      </c>
+      <c r="H82" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J82" s="4">
+        <v>48800</v>
+      </c>
+      <c r="K82" s="4">
+        <v>500</v>
+      </c>
+      <c r="L82" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M82" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N82" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="O82" s="13">
+        <v>0</v>
+      </c>
+      <c r="P82" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>64</v>
+      </c>
+      <c r="R82" s="2">
+        <v>44</v>
+      </c>
+      <c r="S82" s="2">
+        <v>32</v>
+      </c>
+      <c r="T82" s="2">
+        <v>865</v>
+      </c>
+      <c r="U82" s="7">
+        <v>0.54949999999999999</v>
+      </c>
+      <c r="V82" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W82" s="1"/>
+      <c r="X82" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6915,16 +7070,16 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="R2:R80">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+  <conditionalFormatting sqref="R2:R82">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
pre-determined order for model training, with extra training/testing resutls
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9807ABA-9F92-4AFB-ABB0-12C38999EBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98410639-CC25-4946-BD54-014D106B1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="116">
   <si>
     <t>test number</t>
   </si>
@@ -372,6 +372,82 @@
   </si>
   <si>
     <t>best_model_040.pth</t>
+  </si>
+  <si>
+    <t>set order of classes to analyse. Look at
+folder_order.txt for more details</t>
+  </si>
+  <si>
+    <t>best_model_041.pth</t>
+  </si>
+  <si>
+    <t>500 (37)</t>
+  </si>
+  <si>
+    <t>best_model_042.pth</t>
+  </si>
+  <si>
+    <t>best_model_043.pth</t>
+  </si>
+  <si>
+    <t>500 (47)</t>
+  </si>
+  <si>
+    <t>500 (51)</t>
+  </si>
+  <si>
+    <t>best_model_044.pth</t>
+  </si>
+  <si>
+    <t>shuffling of training data every epoch</t>
+  </si>
+  <si>
+    <t>best_model_045.pth</t>
+  </si>
+  <si>
+    <t>500 (81)</t>
+  </si>
+  <si>
+    <t>shuffling of batch data every epoch</t>
+  </si>
+  <si>
+    <t>best_model_046.pth</t>
+  </si>
+  <si>
+    <t>500 (69)</t>
+  </si>
+  <si>
+    <t>500 (94)</t>
+  </si>
+  <si>
+    <t>500 (59)</t>
+  </si>
+  <si>
+    <t>best_model_047.pth</t>
+  </si>
+  <si>
+    <t>500 (60)</t>
+  </si>
+  <si>
+    <t>best_model_048.pth</t>
+  </si>
+  <si>
+    <t>best_model_049.pth</t>
+  </si>
+  <si>
+    <t>best_model_050.pth</t>
+  </si>
+  <si>
+    <t>best_model_051.pth</t>
+  </si>
+  <si>
+    <t>best_model_052.pth</t>
+  </si>
+  <si>
+    <t>best_model_053.pth</t>
+  </si>
+  <si>
+    <t>best_model_054.pth</t>
   </si>
 </sst>
 </file>
@@ -452,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,20 +563,86 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -830,36 +972,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X82" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A2:X82" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X96" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A2:X96" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:X76">
     <sortCondition ref="B2:B80"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="30"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="28"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="39"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="37"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="35"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="34"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="32"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="21"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1162,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:X82"/>
+  <dimension ref="A1:X96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K70" workbookViewId="0">
-      <selection activeCell="U82" sqref="U82"/>
+    <sheetView tabSelected="1" topLeftCell="K76" workbookViewId="0">
+      <selection activeCell="X97" sqref="X97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,27 +1338,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6922,25 +7064,25 @@
       <c r="A81" s="1">
         <v>77</v>
       </c>
-      <c r="B81" s="13">
+      <c r="B81" s="1">
         <v>200</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="13">
+      <c r="E81" s="1">
         <v>2</v>
       </c>
       <c r="F81" s="1">
         <v>0</v>
       </c>
-      <c r="G81" s="13">
-        <v>0</v>
-      </c>
-      <c r="H81" s="13">
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1">
         <v>0.2</v>
       </c>
       <c r="I81" s="1" t="s">
@@ -6949,25 +7091,25 @@
       <c r="J81" s="4">
         <v>108400</v>
       </c>
-      <c r="K81" s="14" t="s">
+      <c r="K81" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="L81" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M81" s="13" t="s">
+      <c r="L81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M81" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N81" s="13">
+      <c r="N81" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O81" s="13">
-        <v>0</v>
-      </c>
-      <c r="P81" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q81" s="13">
+      <c r="O81" s="1">
+        <v>0</v>
+      </c>
+      <c r="P81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="1">
         <v>64</v>
       </c>
       <c r="R81" s="2">
@@ -6999,22 +7141,22 @@
       <c r="B82" s="4">
         <v>100</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D82" s="13" t="s">
+      <c r="D82" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E82" s="13">
+      <c r="E82" s="1">
         <v>2</v>
       </c>
       <c r="F82" s="4">
         <v>100</v>
       </c>
-      <c r="G82" s="13">
-        <v>0</v>
-      </c>
-      <c r="H82" s="13">
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1">
         <v>0.2</v>
       </c>
       <c r="I82" s="1" t="s">
@@ -7026,22 +7168,22 @@
       <c r="K82" s="4">
         <v>500</v>
       </c>
-      <c r="L82" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M82" s="13" t="s">
+      <c r="L82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M82" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N82" s="13">
+      <c r="N82" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O82" s="13">
-        <v>0</v>
-      </c>
-      <c r="P82" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="13">
+      <c r="O82" s="1">
+        <v>0</v>
+      </c>
+      <c r="P82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
         <v>64</v>
       </c>
       <c r="R82" s="2">
@@ -7062,6 +7204,1015 @@
       <c r="W82" s="1"/>
       <c r="X82" s="2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>79</v>
+      </c>
+      <c r="B83" s="14">
+        <v>100</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E83" s="14">
+        <v>2</v>
+      </c>
+      <c r="F83" s="1">
+        <v>100</v>
+      </c>
+      <c r="G83" s="14">
+        <v>0</v>
+      </c>
+      <c r="H83" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J83" s="4">
+        <v>66400</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L83" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M83" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N83" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O83" s="14">
+        <v>0</v>
+      </c>
+      <c r="P83" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="14">
+        <v>64</v>
+      </c>
+      <c r="R83" s="2">
+        <v>34</v>
+      </c>
+      <c r="S83" s="2">
+        <v>27.32</v>
+      </c>
+      <c r="T83" s="2">
+        <v>207</v>
+      </c>
+      <c r="U83" s="7">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="V83" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W83" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="X83" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>80</v>
+      </c>
+      <c r="B84" s="14">
+        <v>100</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E84" s="14">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1">
+        <v>100</v>
+      </c>
+      <c r="G84" s="14">
+        <v>0</v>
+      </c>
+      <c r="H84" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J84" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N84" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O84" s="14">
+        <v>0</v>
+      </c>
+      <c r="P84" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="4">
+        <v>128</v>
+      </c>
+      <c r="R84" s="2">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="S84" s="2">
+        <v>28.02</v>
+      </c>
+      <c r="T84" s="2">
+        <v>228</v>
+      </c>
+      <c r="U84" s="7">
+        <v>0.51359999999999995</v>
+      </c>
+      <c r="V84" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W84" s="1"/>
+      <c r="X84" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>81</v>
+      </c>
+      <c r="B85" s="14">
+        <v>100</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E85" s="14">
+        <v>2</v>
+      </c>
+      <c r="F85" s="1">
+        <v>100</v>
+      </c>
+      <c r="G85" s="14">
+        <v>0</v>
+      </c>
+      <c r="H85" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J85" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N85" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O85" s="14">
+        <v>0</v>
+      </c>
+      <c r="P85" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="4">
+        <v>256</v>
+      </c>
+      <c r="R85" s="2">
+        <v>35.33</v>
+      </c>
+      <c r="S85" s="2">
+        <v>27.53</v>
+      </c>
+      <c r="T85" s="2">
+        <v>227</v>
+      </c>
+      <c r="U85" s="7">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="V85" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W85" s="1"/>
+      <c r="X85" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>82</v>
+      </c>
+      <c r="B86" s="14">
+        <v>100</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E86" s="14">
+        <v>2</v>
+      </c>
+      <c r="F86" s="1">
+        <v>100</v>
+      </c>
+      <c r="G86" s="14">
+        <v>0</v>
+      </c>
+      <c r="H86" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J86" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N86" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O86" s="14">
+        <v>0</v>
+      </c>
+      <c r="P86" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="4">
+        <v>1024</v>
+      </c>
+      <c r="R86" s="2">
+        <v>36.54</v>
+      </c>
+      <c r="S86" s="2">
+        <v>27.82</v>
+      </c>
+      <c r="T86" s="2">
+        <v>529</v>
+      </c>
+      <c r="U86" s="7">
+        <v>0.50929999999999997</v>
+      </c>
+      <c r="V86" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W86" s="1"/>
+      <c r="X86" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>83</v>
+      </c>
+      <c r="B87" s="14">
+        <v>100</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E87" s="14">
+        <v>2</v>
+      </c>
+      <c r="F87" s="1">
+        <v>100</v>
+      </c>
+      <c r="G87" s="14">
+        <v>0</v>
+      </c>
+      <c r="H87" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J87" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N87" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O87" s="14">
+        <v>0</v>
+      </c>
+      <c r="P87" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="14">
+        <v>1024</v>
+      </c>
+      <c r="R87" s="2">
+        <v>35.06</v>
+      </c>
+      <c r="S87" s="2">
+        <v>27.18</v>
+      </c>
+      <c r="T87" s="2">
+        <v>447</v>
+      </c>
+      <c r="U87" s="7">
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="V87" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W87" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="X87" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>84</v>
+      </c>
+      <c r="B88" s="14">
+        <v>100</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E88" s="14">
+        <v>2</v>
+      </c>
+      <c r="F88" s="1">
+        <v>100</v>
+      </c>
+      <c r="G88" s="14">
+        <v>0</v>
+      </c>
+      <c r="H88" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J88" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N88" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O88" s="14">
+        <v>0</v>
+      </c>
+      <c r="P88" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q88" s="14">
+        <v>1024</v>
+      </c>
+      <c r="R88" s="15">
+        <v>36.630000000000003</v>
+      </c>
+      <c r="S88" s="2">
+        <v>28.2</v>
+      </c>
+      <c r="T88" s="2">
+        <v>239</v>
+      </c>
+      <c r="U88" s="7">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="V88" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W88" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="X88" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>85</v>
+      </c>
+      <c r="B89" s="14">
+        <v>100</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E89" s="14">
+        <v>2</v>
+      </c>
+      <c r="F89" s="4">
+        <v>0</v>
+      </c>
+      <c r="G89" s="14">
+        <v>0</v>
+      </c>
+      <c r="H89" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J89" s="14">
+        <v>66400</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N89" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O89" s="14">
+        <v>0</v>
+      </c>
+      <c r="P89" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="14">
+        <v>1024</v>
+      </c>
+      <c r="R89" s="2">
+        <v>36.090000000000003</v>
+      </c>
+      <c r="S89" s="2">
+        <v>27.12</v>
+      </c>
+      <c r="T89" s="2">
+        <v>155</v>
+      </c>
+      <c r="U89" s="7">
+        <v>0.49730000000000002</v>
+      </c>
+      <c r="V89" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W89" s="1"/>
+      <c r="X89" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>86</v>
+      </c>
+      <c r="B90" s="14">
+        <v>100</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E90" s="14">
+        <v>2</v>
+      </c>
+      <c r="F90" s="14">
+        <v>0</v>
+      </c>
+      <c r="G90" s="14">
+        <v>0</v>
+      </c>
+      <c r="H90" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J90" s="4">
+        <v>125500</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N90" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O90" s="14">
+        <v>0</v>
+      </c>
+      <c r="P90" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="14">
+        <v>1024</v>
+      </c>
+      <c r="R90" s="2">
+        <v>29.42</v>
+      </c>
+      <c r="S90" s="2">
+        <v>24.51</v>
+      </c>
+      <c r="T90" s="2">
+        <v>352</v>
+      </c>
+      <c r="U90" s="7">
+        <v>0.46060000000000001</v>
+      </c>
+      <c r="V90" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W90" s="1"/>
+      <c r="X90" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>87</v>
+      </c>
+      <c r="B91" s="14">
+        <v>50</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E91" s="14">
+        <v>2</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="14">
+        <v>0</v>
+      </c>
+      <c r="H91" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J91" s="4">
+        <v>31200</v>
+      </c>
+      <c r="K91" s="4">
+        <v>500</v>
+      </c>
+      <c r="L91" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M91" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N91" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O91" s="14">
+        <v>0</v>
+      </c>
+      <c r="P91" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="14">
+        <v>1024</v>
+      </c>
+      <c r="R91" s="2">
+        <v>63.2</v>
+      </c>
+      <c r="S91" s="2">
+        <v>40.61</v>
+      </c>
+      <c r="T91" s="2">
+        <v>299</v>
+      </c>
+      <c r="U91" s="7">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="V91" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W91" s="1"/>
+      <c r="X91" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>88</v>
+      </c>
+      <c r="B92" s="14">
+        <v>50</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E92" s="14">
+        <v>2</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="14">
+        <v>0</v>
+      </c>
+      <c r="H92" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J92" s="14">
+        <v>31200</v>
+      </c>
+      <c r="K92" s="14">
+        <v>500</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N92" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O92" s="14">
+        <v>0</v>
+      </c>
+      <c r="P92" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="4">
+        <v>64</v>
+      </c>
+      <c r="R92" s="2">
+        <v>57.44</v>
+      </c>
+      <c r="S92" s="2">
+        <v>39.54</v>
+      </c>
+      <c r="T92" s="2">
+        <v>671</v>
+      </c>
+      <c r="U92" s="7">
+        <v>0.64119999999999999</v>
+      </c>
+      <c r="V92" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W92" s="1"/>
+      <c r="X92" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>89</v>
+      </c>
+      <c r="B93" s="14">
+        <v>50</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E93" s="14">
+        <v>2</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="14">
+        <v>0</v>
+      </c>
+      <c r="H93" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J93" s="14">
+        <v>31200</v>
+      </c>
+      <c r="K93" s="14">
+        <v>500</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N93" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O93" s="14">
+        <v>0</v>
+      </c>
+      <c r="P93" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="4">
+        <v>512</v>
+      </c>
+      <c r="R93" s="2">
+        <v>62.04</v>
+      </c>
+      <c r="S93" s="2">
+        <v>40.53</v>
+      </c>
+      <c r="T93" s="2">
+        <v>317</v>
+      </c>
+      <c r="U93" s="7">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="V93" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W93" s="1"/>
+      <c r="X93" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>90</v>
+      </c>
+      <c r="B94" s="14">
+        <v>50</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E94" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="14">
+        <v>0</v>
+      </c>
+      <c r="H94" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J94" s="4">
+        <v>42200</v>
+      </c>
+      <c r="K94" s="14">
+        <v>500</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N94" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O94" s="14">
+        <v>0</v>
+      </c>
+      <c r="P94" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="14">
+        <v>512</v>
+      </c>
+      <c r="R94" s="2">
+        <v>46.57</v>
+      </c>
+      <c r="S94" s="2">
+        <v>34.53</v>
+      </c>
+      <c r="T94" s="2">
+        <v>371</v>
+      </c>
+      <c r="U94" s="7">
+        <v>0.59240000000000004</v>
+      </c>
+      <c r="V94" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W94" s="1"/>
+      <c r="X94" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>91</v>
+      </c>
+      <c r="B95" s="14">
+        <v>50</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E95" s="4">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="14">
+        <v>0</v>
+      </c>
+      <c r="H95" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J95" s="4">
+        <v>63850</v>
+      </c>
+      <c r="K95" s="14">
+        <v>500</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N95" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O95" s="14">
+        <v>0</v>
+      </c>
+      <c r="P95" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="14">
+        <v>512</v>
+      </c>
+      <c r="R95" s="2">
+        <v>34.71</v>
+      </c>
+      <c r="S95" s="2">
+        <v>29.49</v>
+      </c>
+      <c r="T95" s="2">
+        <v>515</v>
+      </c>
+      <c r="U95" s="7">
+        <v>0.55089999999999995</v>
+      </c>
+      <c r="V95" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W95" s="1"/>
+      <c r="X95" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B96" s="14"/>
+      <c r="C96" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E96" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="14">
+        <v>0</v>
+      </c>
+      <c r="H96" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J96" s="4">
+        <v>24950</v>
+      </c>
+      <c r="K96" s="14">
+        <v>500</v>
+      </c>
+      <c r="L96" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M96" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N96" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O96" s="14">
+        <v>0</v>
+      </c>
+      <c r="P96" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="14">
+        <v>512</v>
+      </c>
+      <c r="R96" s="2">
+        <v>81.75</v>
+      </c>
+      <c r="S96" s="2">
+        <v>46.19</v>
+      </c>
+      <c r="T96" s="2">
+        <v>258</v>
+      </c>
+      <c r="U96" s="7">
+        <v>0.6593</v>
+      </c>
+      <c r="V96" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W96" s="1"/>
+      <c r="X96" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -7070,16 +8221,16 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="R2:R82">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
+  <conditionalFormatting sqref="R2:R96">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
sequential aggregation successfully tested on all folder files
</commit_message>
<xml_diff>
--- a/code/simple CNN test results.xlsx
+++ b/code/simple CNN test results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98410639-CC25-4946-BD54-014D106B1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256DBEC6-E501-4C6F-8830-670EA93DFFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,122 +569,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <fill>
         <patternFill>
@@ -972,36 +861,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X96" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:X96" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:X96" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:X76">
     <sortCondition ref="B2:B80"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="40"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="39"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="37"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="35"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="34"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="32"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="22"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="21"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="25"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1306,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
   <dimension ref="A1:X96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K76" workbookViewId="0">
-      <selection activeCell="X97" sqref="X97"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7210,25 +7099,25 @@
       <c r="A83" s="1">
         <v>79</v>
       </c>
-      <c r="B83" s="14">
+      <c r="B83" s="1">
         <v>100</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="14">
+      <c r="E83" s="1">
         <v>2</v>
       </c>
       <c r="F83" s="1">
         <v>100</v>
       </c>
-      <c r="G83" s="14">
-        <v>0</v>
-      </c>
-      <c r="H83" s="14">
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
         <v>0.2</v>
       </c>
       <c r="I83" s="1" t="s">
@@ -7240,22 +7129,22 @@
       <c r="K83" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="L83" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M83" s="14" t="s">
+      <c r="L83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M83" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N83" s="14">
+      <c r="N83" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O83" s="14">
-        <v>0</v>
-      </c>
-      <c r="P83" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q83" s="14">
+      <c r="O83" s="1">
+        <v>0</v>
+      </c>
+      <c r="P83" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="1">
         <v>64</v>
       </c>
       <c r="R83" s="2">
@@ -7284,49 +7173,49 @@
       <c r="A84" s="1">
         <v>80</v>
       </c>
-      <c r="B84" s="14">
+      <c r="B84" s="1">
         <v>100</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="14" t="s">
+      <c r="D84" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E84" s="14">
+      <c r="E84" s="1">
         <v>2</v>
       </c>
       <c r="F84" s="1">
         <v>100</v>
       </c>
-      <c r="G84" s="14">
-        <v>0</v>
-      </c>
-      <c r="H84" s="14">
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1">
         <v>0.2</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J84" s="14">
+      <c r="J84" s="1">
         <v>66400</v>
       </c>
       <c r="K84" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="L84" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M84" s="14" t="s">
+      <c r="L84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M84" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N84" s="14">
+      <c r="N84" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O84" s="14">
-        <v>0</v>
-      </c>
-      <c r="P84" s="14">
+      <c r="O84" s="1">
+        <v>0</v>
+      </c>
+      <c r="P84" s="1">
         <v>0</v>
       </c>
       <c r="Q84" s="4">
@@ -7356,49 +7245,49 @@
       <c r="A85" s="1">
         <v>81</v>
       </c>
-      <c r="B85" s="14">
+      <c r="B85" s="1">
         <v>100</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E85" s="14">
+      <c r="E85" s="1">
         <v>2</v>
       </c>
       <c r="F85" s="1">
         <v>100</v>
       </c>
-      <c r="G85" s="14">
-        <v>0</v>
-      </c>
-      <c r="H85" s="14">
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
         <v>0.2</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J85" s="14">
+      <c r="J85" s="1">
         <v>66400</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="L85" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M85" s="14" t="s">
+      <c r="L85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N85" s="14">
+      <c r="N85" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O85" s="14">
-        <v>0</v>
-      </c>
-      <c r="P85" s="14">
+      <c r="O85" s="1">
+        <v>0</v>
+      </c>
+      <c r="P85" s="1">
         <v>0</v>
       </c>
       <c r="Q85" s="4">
@@ -7428,49 +7317,49 @@
       <c r="A86" s="1">
         <v>82</v>
       </c>
-      <c r="B86" s="14">
+      <c r="B86" s="1">
         <v>100</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E86" s="14">
+      <c r="E86" s="1">
         <v>2</v>
       </c>
       <c r="F86" s="1">
         <v>100</v>
       </c>
-      <c r="G86" s="14">
-        <v>0</v>
-      </c>
-      <c r="H86" s="14">
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1">
         <v>0.2</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J86" s="14">
+      <c r="J86" s="1">
         <v>66400</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L86" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M86" s="14" t="s">
+      <c r="L86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M86" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N86" s="14">
+      <c r="N86" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O86" s="14">
-        <v>0</v>
-      </c>
-      <c r="P86" s="14">
+      <c r="O86" s="1">
+        <v>0</v>
+      </c>
+      <c r="P86" s="1">
         <v>0</v>
       </c>
       <c r="Q86" s="4">
@@ -7500,52 +7389,52 @@
       <c r="A87" s="1">
         <v>83</v>
       </c>
-      <c r="B87" s="14">
+      <c r="B87" s="1">
         <v>100</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E87" s="14">
+      <c r="E87" s="1">
         <v>2</v>
       </c>
       <c r="F87" s="1">
         <v>100</v>
       </c>
-      <c r="G87" s="14">
-        <v>0</v>
-      </c>
-      <c r="H87" s="14">
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="1">
         <v>0.2</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J87" s="14">
+      <c r="J87" s="1">
         <v>66400</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L87" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M87" s="14" t="s">
+      <c r="L87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M87" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N87" s="14">
+      <c r="N87" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O87" s="14">
-        <v>0</v>
-      </c>
-      <c r="P87" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="14">
+      <c r="O87" s="1">
+        <v>0</v>
+      </c>
+      <c r="P87" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="1">
         <v>1024</v>
       </c>
       <c r="R87" s="2">
@@ -7574,55 +7463,55 @@
       <c r="A88" s="1">
         <v>84</v>
       </c>
-      <c r="B88" s="14">
+      <c r="B88" s="1">
         <v>100</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C88" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E88" s="14">
+      <c r="E88" s="1">
         <v>2</v>
       </c>
       <c r="F88" s="1">
         <v>100</v>
       </c>
-      <c r="G88" s="14">
-        <v>0</v>
-      </c>
-      <c r="H88" s="14">
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1">
         <v>0.2</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J88" s="14">
+      <c r="J88" s="1">
         <v>66400</v>
       </c>
       <c r="K88" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="L88" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M88" s="14" t="s">
+      <c r="L88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M88" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N88" s="14">
+      <c r="N88" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O88" s="14">
-        <v>0</v>
-      </c>
-      <c r="P88" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q88" s="14">
+      <c r="O88" s="1">
+        <v>0</v>
+      </c>
+      <c r="P88" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q88" s="1">
         <v>1024</v>
       </c>
-      <c r="R88" s="15">
+      <c r="R88" s="2">
         <v>36.630000000000003</v>
       </c>
       <c r="S88" s="2">
@@ -7648,52 +7537,52 @@
       <c r="A89" s="1">
         <v>85</v>
       </c>
-      <c r="B89" s="14">
+      <c r="B89" s="1">
         <v>100</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C89" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E89" s="14">
+      <c r="E89" s="1">
         <v>2</v>
       </c>
       <c r="F89" s="4">
         <v>0</v>
       </c>
-      <c r="G89" s="14">
-        <v>0</v>
-      </c>
-      <c r="H89" s="14">
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
         <v>0.2</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J89" s="14">
+      <c r="J89" s="1">
         <v>66400</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="L89" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M89" s="14" t="s">
+      <c r="L89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M89" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N89" s="14">
+      <c r="N89" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O89" s="14">
-        <v>0</v>
-      </c>
-      <c r="P89" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q89" s="14">
+      <c r="O89" s="1">
+        <v>0</v>
+      </c>
+      <c r="P89" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="1">
         <v>1024</v>
       </c>
       <c r="R89" s="2">
@@ -7720,25 +7609,25 @@
       <c r="A90" s="1">
         <v>86</v>
       </c>
-      <c r="B90" s="14">
+      <c r="B90" s="1">
         <v>100</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E90" s="14">
-        <v>2</v>
-      </c>
-      <c r="F90" s="14">
-        <v>0</v>
-      </c>
-      <c r="G90" s="14">
-        <v>0</v>
-      </c>
-      <c r="H90" s="14">
+      <c r="E90" s="1">
+        <v>2</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0</v>
+      </c>
+      <c r="H90" s="1">
         <v>0.2</v>
       </c>
       <c r="I90" s="1" t="s">
@@ -7750,22 +7639,22 @@
       <c r="K90" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L90" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M90" s="14" t="s">
+      <c r="L90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M90" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N90" s="14">
+      <c r="N90" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O90" s="14">
-        <v>0</v>
-      </c>
-      <c r="P90" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="14">
+      <c r="O90" s="1">
+        <v>0</v>
+      </c>
+      <c r="P90" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="1">
         <v>1024</v>
       </c>
       <c r="R90" s="2">
@@ -7792,25 +7681,25 @@
       <c r="A91" s="1">
         <v>87</v>
       </c>
-      <c r="B91" s="14">
+      <c r="B91" s="1">
         <v>50</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E91" s="14">
+      <c r="E91" s="1">
         <v>2</v>
       </c>
       <c r="F91" s="1">
         <v>0</v>
       </c>
-      <c r="G91" s="14">
-        <v>0</v>
-      </c>
-      <c r="H91" s="14">
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1">
         <v>0.2</v>
       </c>
       <c r="I91" s="1" t="s">
@@ -7822,22 +7711,22 @@
       <c r="K91" s="4">
         <v>500</v>
       </c>
-      <c r="L91" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M91" s="14" t="s">
+      <c r="L91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M91" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N91" s="14">
+      <c r="N91" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O91" s="14">
-        <v>0</v>
-      </c>
-      <c r="P91" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q91" s="14">
+      <c r="O91" s="1">
+        <v>0</v>
+      </c>
+      <c r="P91" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="1">
         <v>1024</v>
       </c>
       <c r="R91" s="2">
@@ -7864,49 +7753,49 @@
       <c r="A92" s="1">
         <v>88</v>
       </c>
-      <c r="B92" s="14">
+      <c r="B92" s="1">
         <v>50</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C92" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E92" s="14">
+      <c r="E92" s="1">
         <v>2</v>
       </c>
       <c r="F92" s="1">
         <v>0</v>
       </c>
-      <c r="G92" s="14">
-        <v>0</v>
-      </c>
-      <c r="H92" s="14">
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
         <v>0.2</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J92" s="14">
+      <c r="J92" s="1">
         <v>31200</v>
       </c>
-      <c r="K92" s="14">
+      <c r="K92" s="1">
         <v>500</v>
       </c>
-      <c r="L92" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M92" s="14" t="s">
+      <c r="L92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M92" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N92" s="14">
+      <c r="N92" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O92" s="14">
-        <v>0</v>
-      </c>
-      <c r="P92" s="14">
+      <c r="O92" s="1">
+        <v>0</v>
+      </c>
+      <c r="P92" s="1">
         <v>0</v>
       </c>
       <c r="Q92" s="4">
@@ -7936,49 +7825,49 @@
       <c r="A93" s="1">
         <v>89</v>
       </c>
-      <c r="B93" s="14">
+      <c r="B93" s="1">
         <v>50</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D93" s="14" t="s">
+      <c r="D93" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E93" s="14">
+      <c r="E93" s="1">
         <v>2</v>
       </c>
       <c r="F93" s="1">
         <v>0</v>
       </c>
-      <c r="G93" s="14">
-        <v>0</v>
-      </c>
-      <c r="H93" s="14">
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
         <v>0.2</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J93" s="14">
+      <c r="J93" s="1">
         <v>31200</v>
       </c>
-      <c r="K93" s="14">
+      <c r="K93" s="1">
         <v>500</v>
       </c>
-      <c r="L93" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M93" s="14" t="s">
+      <c r="L93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M93" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N93" s="14">
+      <c r="N93" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O93" s="14">
-        <v>0</v>
-      </c>
-      <c r="P93" s="14">
+      <c r="O93" s="1">
+        <v>0</v>
+      </c>
+      <c r="P93" s="1">
         <v>0</v>
       </c>
       <c r="Q93" s="4">
@@ -8008,13 +7897,13 @@
       <c r="A94" s="1">
         <v>90</v>
       </c>
-      <c r="B94" s="14">
+      <c r="B94" s="1">
         <v>50</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C94" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D94" s="14" t="s">
+      <c r="D94" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E94" s="4">
@@ -8023,10 +7912,10 @@
       <c r="F94" s="1">
         <v>0</v>
       </c>
-      <c r="G94" s="14">
-        <v>0</v>
-      </c>
-      <c r="H94" s="14">
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
         <v>0.2</v>
       </c>
       <c r="I94" s="1" t="s">
@@ -8035,25 +7924,25 @@
       <c r="J94" s="4">
         <v>42200</v>
       </c>
-      <c r="K94" s="14">
+      <c r="K94" s="1">
         <v>500</v>
       </c>
-      <c r="L94" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M94" s="14" t="s">
+      <c r="L94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M94" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N94" s="14">
+      <c r="N94" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O94" s="14">
-        <v>0</v>
-      </c>
-      <c r="P94" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="14">
+      <c r="O94" s="1">
+        <v>0</v>
+      </c>
+      <c r="P94" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="1">
         <v>512</v>
       </c>
       <c r="R94" s="2">
@@ -8080,13 +7969,13 @@
       <c r="A95" s="1">
         <v>91</v>
       </c>
-      <c r="B95" s="14">
+      <c r="B95" s="1">
         <v>50</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C95" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E95" s="4">
@@ -8095,10 +7984,10 @@
       <c r="F95" s="1">
         <v>0</v>
       </c>
-      <c r="G95" s="14">
-        <v>0</v>
-      </c>
-      <c r="H95" s="14">
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+      <c r="H95" s="1">
         <v>0.2</v>
       </c>
       <c r="I95" s="1" t="s">
@@ -8107,25 +7996,25 @@
       <c r="J95" s="4">
         <v>63850</v>
       </c>
-      <c r="K95" s="14">
+      <c r="K95" s="1">
         <v>500</v>
       </c>
-      <c r="L95" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M95" s="14" t="s">
+      <c r="L95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N95" s="14">
+      <c r="N95" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O95" s="14">
-        <v>0</v>
-      </c>
-      <c r="P95" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="14">
+      <c r="O95" s="1">
+        <v>0</v>
+      </c>
+      <c r="P95" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="1">
         <v>512</v>
       </c>
       <c r="R95" s="2">
@@ -8149,11 +8038,16 @@
       </c>
     </row>
     <row r="96" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B96" s="14"/>
-      <c r="C96" s="14" t="s">
+      <c r="A96" s="1">
+        <v>92</v>
+      </c>
+      <c r="B96" s="1">
+        <v>50</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E96" s="4">
@@ -8162,10 +8056,10 @@
       <c r="F96" s="1">
         <v>0</v>
       </c>
-      <c r="G96" s="14">
-        <v>0</v>
-      </c>
-      <c r="H96" s="14">
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
         <v>0.2</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -8174,25 +8068,25 @@
       <c r="J96" s="4">
         <v>24950</v>
       </c>
-      <c r="K96" s="14">
+      <c r="K96" s="1">
         <v>500</v>
       </c>
-      <c r="L96" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M96" s="14" t="s">
+      <c r="L96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M96" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N96" s="14">
+      <c r="N96" s="1">
         <v>1E-3</v>
       </c>
-      <c r="O96" s="14">
-        <v>0</v>
-      </c>
-      <c r="P96" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="14">
+      <c r="O96" s="1">
+        <v>0</v>
+      </c>
+      <c r="P96" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="1">
         <v>512</v>
       </c>
       <c r="R96" s="2">
@@ -8222,15 +8116,15 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="R2:R96">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>